<commit_message>
best contracts menu yet + a lot more contracts
</commit_message>
<xml_diff>
--- a/assets/contracts and data.xlsx
+++ b/assets/contracts and data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\link-builder\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96916315-A2DD-4816-BC5E-88F6A31D9AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF1B08F-B50A-446C-84EB-333BF4AA30B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Health Insurance</t>
   </si>
   <si>
-    <t>Flight Insurance</t>
-  </si>
-  <si>
     <t>Cloud Downtime</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Cerberus Wallet 2FA</t>
+  </si>
+  <si>
+    <t>Etherisc Flight Insurance</t>
   </si>
 </sst>
 </file>
@@ -327,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -385,11 +385,29 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -723,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ67"/>
+  <dimension ref="A1:AQ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,64 +789,64 @@
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="N1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="V1" s="8" t="s">
         <v>9</v>
@@ -837,28 +855,28 @@
         <v>10</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Y1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB1" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>12</v>
@@ -870,10 +888,10 @@
         <v>14</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
@@ -884,7 +902,7 @@
     </row>
     <row r="2" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -931,17 +949,17 @@
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="13"/>
@@ -984,11 +1002,11 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -1033,12 +1051,12 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="13"/>
       <c r="D5" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="18"/>
@@ -1082,7 +1100,7 @@
     </row>
     <row r="6" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -1133,13 +1151,13 @@
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="19"/>
       <c r="G7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="19"/>
@@ -1150,17 +1168,17 @@
       <c r="N7" s="17"/>
       <c r="O7" s="19"/>
       <c r="P7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S7" s="17"/>
       <c r="T7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U7" s="19"/>
       <c r="V7" s="17"/>
@@ -1188,18 +1206,18 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="19"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="17"/>
@@ -1209,17 +1227,17 @@
       <c r="N8" s="17"/>
       <c r="O8" s="19"/>
       <c r="P8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S8" s="17"/>
       <c r="T8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U8" s="19"/>
       <c r="V8" s="17"/>
@@ -1247,7 +1265,7 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="17"/>
@@ -1255,13 +1273,13 @@
       <c r="E9" s="17"/>
       <c r="F9" s="19"/>
       <c r="G9" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="19"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
@@ -1298,7 +1316,7 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="17"/>
@@ -1309,7 +1327,7 @@
       <c r="H10" s="17"/>
       <c r="I10" s="19"/>
       <c r="J10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -1317,17 +1335,17 @@
       <c r="N10" s="17"/>
       <c r="O10" s="19"/>
       <c r="P10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S10" s="17"/>
       <c r="T10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U10" s="19"/>
       <c r="V10" s="17"/>
@@ -1354,18 +1372,18 @@
       <c r="AQ10" s="15"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>53</v>
+      <c r="A11" s="24" t="s">
+        <v>52</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="17"/>
@@ -1407,12 +1425,12 @@
       <c r="AQ11" s="15"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>54</v>
+      <c r="A12" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -1427,17 +1445,17 @@
       <c r="N12" s="17"/>
       <c r="O12" s="19"/>
       <c r="P12" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S12" s="17"/>
       <c r="T12" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U12" s="19"/>
       <c r="V12" s="17"/>
@@ -1465,7 +1483,7 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="17"/>
@@ -1479,10 +1497,10 @@
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
       <c r="M13" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O13" s="19"/>
       <c r="P13" s="17"/>
@@ -1516,7 +1534,7 @@
     </row>
     <row r="14" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -1563,17 +1581,17 @@
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="13"/>
@@ -1615,18 +1633,18 @@
       <c r="AQ15" s="15"/>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>44</v>
+      <c r="A16" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="17"/>
@@ -1669,17 +1687,17 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="17"/>
@@ -1721,18 +1739,18 @@
       <c r="AQ17" s="15"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>40</v>
+      <c r="A18" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="17"/>
@@ -1774,18 +1792,18 @@
       <c r="AQ18" s="15"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>41</v>
+      <c r="A19" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="17"/>
@@ -1828,17 +1846,17 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="17"/>
@@ -1885,13 +1903,13 @@
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="17"/>
@@ -1908,14 +1926,14 @@
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
       <c r="T21" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U21" s="19"/>
       <c r="V21" s="17"/>
       <c r="W21" s="17"/>
       <c r="X21" s="17"/>
       <c r="Y21" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Z21" s="17"/>
       <c r="AA21" s="17"/>
@@ -1937,18 +1955,18 @@
       <c r="AQ21" s="15"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
+      <c r="A22" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="17"/>
@@ -1957,13 +1975,13 @@
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O22" s="19"/>
       <c r="P22" s="17"/>
@@ -1977,7 +1995,7 @@
       <c r="X22" s="17"/>
       <c r="Y22" s="17"/>
       <c r="Z22" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA22" s="17"/>
       <c r="AB22" s="19"/>
@@ -1997,109 +2015,109 @@
       <c r="AP22" s="15"/>
       <c r="AQ22" s="15"/>
     </row>
-    <row r="23" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>37</v>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>5</v>
       </c>
       <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
       <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" s="17"/>
       <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19"/>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="17"/>
+      <c r="AA23" s="17"/>
       <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="19"/>
-      <c r="AH23" s="19"/>
-      <c r="AI23" s="19"/>
-      <c r="AJ23" s="19"/>
-      <c r="AK23" s="23"/>
-      <c r="AL23" s="23"/>
-      <c r="AM23" s="23"/>
-      <c r="AN23" s="23"/>
-      <c r="AO23" s="23"/>
-      <c r="AP23" s="23"/>
-      <c r="AQ23" s="23"/>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="AC23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD23" s="17"/>
+      <c r="AE23" s="17"/>
+      <c r="AF23" s="17"/>
+      <c r="AG23" s="17"/>
+      <c r="AH23" s="17"/>
+      <c r="AI23" s="17"/>
+      <c r="AJ23" s="17"/>
+      <c r="AK23" s="15"/>
+      <c r="AL23" s="15"/>
+      <c r="AM23" s="15"/>
+      <c r="AN23" s="15"/>
+      <c r="AO23" s="15"/>
+      <c r="AP23" s="15"/>
+      <c r="AQ23" s="15"/>
+    </row>
+    <row r="24" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="19"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
+      <c r="AG24" s="19"/>
+      <c r="AH24" s="19"/>
+      <c r="AI24" s="19"/>
+      <c r="AJ24" s="19"/>
+      <c r="AK24" s="23"/>
+      <c r="AL24" s="23"/>
+      <c r="AM24" s="23"/>
+      <c r="AN24" s="23"/>
+      <c r="AO24" s="23"/>
+      <c r="AP24" s="23"/>
+      <c r="AQ24" s="23"/>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
         <v>1</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="T24" s="17"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="17"/>
-      <c r="W24" s="17"/>
-      <c r="X24" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="17"/>
-      <c r="AA24" s="17"/>
-      <c r="AB24" s="19"/>
-      <c r="AC24" s="17"/>
-      <c r="AD24" s="17"/>
-      <c r="AE24" s="17"/>
-      <c r="AF24" s="17"/>
-      <c r="AG24" s="17"/>
-      <c r="AH24" s="17"/>
-      <c r="AI24" s="17"/>
-      <c r="AJ24" s="17"/>
-      <c r="AK24" s="15"/>
-      <c r="AL24" s="15"/>
-      <c r="AM24" s="15"/>
-      <c r="AN24" s="15"/>
-      <c r="AO24" s="15"/>
-      <c r="AP24" s="15"/>
-      <c r="AQ24" s="15"/>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="17"/>
@@ -2112,7 +2130,7 @@
       <c r="J25" s="17"/>
       <c r="K25" s="17"/>
       <c r="L25" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
@@ -2121,13 +2139,15 @@
       <c r="Q25" s="17"/>
       <c r="R25" s="17"/>
       <c r="S25" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T25" s="17"/>
       <c r="U25" s="19"/>
       <c r="V25" s="17"/>
       <c r="W25" s="17"/>
-      <c r="X25" s="17"/>
+      <c r="X25" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="Y25" s="17"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="17"/>
@@ -2135,9 +2155,7 @@
       <c r="AC25" s="17"/>
       <c r="AD25" s="17"/>
       <c r="AE25" s="17"/>
-      <c r="AF25" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="AF25" s="17"/>
       <c r="AG25" s="17"/>
       <c r="AH25" s="17"/>
       <c r="AI25" s="17"/>
@@ -2151,8 +2169,8 @@
       <c r="AQ25" s="15"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>51</v>
+      <c r="A26" s="24" t="s">
+        <v>2</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="17"/>
@@ -2165,7 +2183,7 @@
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
@@ -2174,13 +2192,11 @@
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
       <c r="S26" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T26" s="17"/>
       <c r="U26" s="19"/>
-      <c r="V26" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="V26" s="17"/>
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
       <c r="Y26" s="17"/>
@@ -2190,7 +2206,9 @@
       <c r="AC26" s="17"/>
       <c r="AD26" s="17"/>
       <c r="AE26" s="17"/>
-      <c r="AF26" s="17"/>
+      <c r="AF26" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AG26" s="17"/>
       <c r="AH26" s="17"/>
       <c r="AI26" s="17"/>
@@ -2204,8 +2222,8 @@
       <c r="AQ26" s="15"/>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>3</v>
+      <c r="A27" s="24" t="s">
+        <v>50</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="17"/>
@@ -2218,7 +2236,7 @@
       <c r="J27" s="17"/>
       <c r="K27" s="17"/>
       <c r="L27" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
@@ -2227,11 +2245,13 @@
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
       <c r="S27" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T27" s="17"/>
       <c r="U27" s="19"/>
-      <c r="V27" s="17"/>
+      <c r="V27" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="W27" s="17"/>
       <c r="X27" s="17"/>
       <c r="Y27" s="17"/>
@@ -2244,9 +2264,7 @@
       <c r="AF27" s="17"/>
       <c r="AG27" s="17"/>
       <c r="AH27" s="17"/>
-      <c r="AI27" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="AI27" s="17"/>
       <c r="AJ27" s="17"/>
       <c r="AK27" s="15"/>
       <c r="AL27" s="15"/>
@@ -2257,8 +2275,8 @@
       <c r="AQ27" s="15"/>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>16</v>
+      <c r="A28" s="24" t="s">
+        <v>3</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="17"/>
@@ -2271,7 +2289,7 @@
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
       <c r="L28" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
@@ -2280,7 +2298,7 @@
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
       <c r="S28" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T28" s="17"/>
       <c r="U28" s="19"/>
@@ -2289,9 +2307,7 @@
       <c r="X28" s="17"/>
       <c r="Y28" s="17"/>
       <c r="Z28" s="17"/>
-      <c r="AA28" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="AA28" s="17"/>
       <c r="AB28" s="19"/>
       <c r="AC28" s="17"/>
       <c r="AD28" s="17"/>
@@ -2299,7 +2315,9 @@
       <c r="AF28" s="17"/>
       <c r="AG28" s="17"/>
       <c r="AH28" s="17"/>
-      <c r="AI28" s="17"/>
+      <c r="AI28" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AJ28" s="17"/>
       <c r="AK28" s="15"/>
       <c r="AL28" s="15"/>
@@ -2311,7 +2329,7 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="17"/>
@@ -2324,7 +2342,7 @@
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
@@ -2333,7 +2351,7 @@
       <c r="Q29" s="17"/>
       <c r="R29" s="17"/>
       <c r="S29" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T29" s="17"/>
       <c r="U29" s="19"/>
@@ -2342,12 +2360,12 @@
       <c r="X29" s="17"/>
       <c r="Y29" s="17"/>
       <c r="Z29" s="17"/>
-      <c r="AA29" s="17"/>
+      <c r="AA29" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AB29" s="19"/>
       <c r="AC29" s="17"/>
-      <c r="AD29" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="AD29" s="17"/>
       <c r="AE29" s="17"/>
       <c r="AF29" s="17"/>
       <c r="AG29" s="17"/>
@@ -2364,7 +2382,7 @@
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="17"/>
@@ -2377,7 +2395,7 @@
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
       <c r="L30" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
@@ -2386,7 +2404,7 @@
       <c r="Q30" s="17"/>
       <c r="R30" s="17"/>
       <c r="S30" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T30" s="17"/>
       <c r="U30" s="19"/>
@@ -2398,10 +2416,10 @@
       <c r="AA30" s="17"/>
       <c r="AB30" s="19"/>
       <c r="AC30" s="17"/>
-      <c r="AD30" s="17"/>
-      <c r="AE30" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="AD30" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE30" s="17"/>
       <c r="AF30" s="17"/>
       <c r="AG30" s="17"/>
       <c r="AH30" s="17"/>
@@ -2415,9 +2433,9 @@
       <c r="AP30" s="15"/>
       <c r="AQ30" s="15"/>
     </row>
-    <row r="31" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="17"/>
@@ -2430,7 +2448,7 @@
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
       <c r="L31" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
@@ -2438,7 +2456,9 @@
       <c r="P31" s="17"/>
       <c r="Q31" s="17"/>
       <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
+      <c r="S31" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="T31" s="17"/>
       <c r="U31" s="19"/>
       <c r="V31" s="17"/>
@@ -2450,14 +2470,14 @@
       <c r="AB31" s="19"/>
       <c r="AC31" s="17"/>
       <c r="AD31" s="17"/>
-      <c r="AE31" s="17"/>
+      <c r="AE31" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AF31" s="17"/>
       <c r="AG31" s="17"/>
       <c r="AH31" s="17"/>
       <c r="AI31" s="17"/>
-      <c r="AJ31" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="AJ31" s="17"/>
       <c r="AK31" s="15"/>
       <c r="AL31" s="15"/>
       <c r="AM31" s="15"/>
@@ -2468,7 +2488,7 @@
     </row>
     <row r="32" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="17"/>
@@ -2481,7 +2501,7 @@
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
       <c r="L32" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
@@ -2489,9 +2509,7 @@
       <c r="P32" s="17"/>
       <c r="Q32" s="17"/>
       <c r="R32" s="17"/>
-      <c r="S32" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="S32" s="17"/>
       <c r="T32" s="17"/>
       <c r="U32" s="19"/>
       <c r="V32" s="17"/>
@@ -2508,7 +2526,9 @@
       <c r="AG32" s="17"/>
       <c r="AH32" s="17"/>
       <c r="AI32" s="17"/>
-      <c r="AJ32" s="17"/>
+      <c r="AJ32" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AK32" s="15"/>
       <c r="AL32" s="15"/>
       <c r="AM32" s="15"/>
@@ -2531,14 +2551,18 @@
       <c r="I33" s="19"/>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
+      <c r="L33" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
       <c r="O33" s="19"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="17"/>
       <c r="R33" s="17"/>
-      <c r="S33" s="17"/>
+      <c r="S33" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="T33" s="17"/>
       <c r="U33" s="19"/>
       <c r="V33" s="17"/>
@@ -2564,9 +2588,9 @@
       <c r="AP33" s="15"/>
       <c r="AQ33" s="15"/>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="17"/>
@@ -2578,9 +2602,7 @@
       <c r="I34" s="19"/>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
-      <c r="L34" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="L34" s="17"/>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
       <c r="O34" s="19"/>
@@ -2615,7 +2637,7 @@
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="17"/>
@@ -2628,7 +2650,7 @@
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
       <c r="L35" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -2636,9 +2658,7 @@
       <c r="P35" s="17"/>
       <c r="Q35" s="17"/>
       <c r="R35" s="17"/>
-      <c r="S35" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="S35" s="17"/>
       <c r="T35" s="17"/>
       <c r="U35" s="19"/>
       <c r="V35" s="17"/>
@@ -2648,9 +2668,7 @@
       <c r="Z35" s="17"/>
       <c r="AA35" s="17"/>
       <c r="AB35" s="19"/>
-      <c r="AC35" s="17" t="s">
-        <v>23</v>
-      </c>
+      <c r="AC35" s="17"/>
       <c r="AD35" s="17"/>
       <c r="AE35" s="17"/>
       <c r="AF35" s="17"/>
@@ -2667,7 +2685,8 @@
       <c r="AQ35" s="15"/>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="18"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
@@ -3635,41 +3654,48 @@
       <c r="AQ57" s="15"/>
     </row>
     <row r="58" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B58" s="20"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
-      <c r="O58" s="20"/>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-      <c r="R58" s="2"/>
-      <c r="S58" s="2"/>
-      <c r="T58" s="2"/>
-      <c r="U58" s="20"/>
-      <c r="V58" s="2"/>
-      <c r="W58" s="2"/>
-      <c r="X58" s="2"/>
-      <c r="Y58" s="2"/>
-      <c r="Z58" s="2"/>
-      <c r="AA58" s="2"/>
-      <c r="AB58" s="20"/>
-      <c r="AC58" s="2"/>
-      <c r="AD58" s="2"/>
-      <c r="AE58" s="2"/>
-      <c r="AF58" s="2"/>
-      <c r="AG58" s="2"/>
-      <c r="AH58" s="2"/>
-      <c r="AI58" s="2"/>
-      <c r="AJ58" s="2"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="19"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="17"/>
+      <c r="U58" s="19"/>
+      <c r="V58" s="17"/>
+      <c r="W58" s="17"/>
+      <c r="X58" s="17"/>
+      <c r="Y58" s="17"/>
+      <c r="Z58" s="17"/>
+      <c r="AA58" s="17"/>
+      <c r="AB58" s="19"/>
+      <c r="AC58" s="17"/>
+      <c r="AD58" s="17"/>
+      <c r="AE58" s="17"/>
+      <c r="AF58" s="17"/>
+      <c r="AG58" s="17"/>
+      <c r="AH58" s="17"/>
+      <c r="AI58" s="17"/>
+      <c r="AJ58" s="17"/>
+      <c r="AK58" s="15"/>
+      <c r="AL58" s="15"/>
+      <c r="AM58" s="15"/>
+      <c r="AN58" s="15"/>
+      <c r="AO58" s="15"/>
+      <c r="AP58" s="15"/>
+      <c r="AQ58" s="15"/>
     </row>
     <row r="59" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B59" s="20"/>
@@ -4004,39 +4030,86 @@
       <c r="AI67" s="2"/>
       <c r="AJ67" s="2"/>
     </row>
+    <row r="68" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B68" s="20"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="20"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+      <c r="U68" s="20"/>
+      <c r="V68" s="2"/>
+      <c r="W68" s="2"/>
+      <c r="X68" s="2"/>
+      <c r="Y68" s="2"/>
+      <c r="Z68" s="2"/>
+      <c r="AA68" s="2"/>
+      <c r="AB68" s="20"/>
+      <c r="AC68" s="2"/>
+      <c r="AD68" s="2"/>
+      <c r="AE68" s="2"/>
+      <c r="AF68" s="2"/>
+      <c r="AG68" s="2"/>
+      <c r="AH68" s="2"/>
+      <c r="AI68" s="2"/>
+      <c r="AJ68" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:AJ67">
-    <cfRule type="cellIs" dxfId="6" priority="17" operator="equal">
+  <conditionalFormatting sqref="B2:AJ22 B24:AJ68">
+    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P10:R13 P16:R35 X16:X35">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+  <conditionalFormatting sqref="P10:R13 P16:R22 X16:X22 X24:X36 P24:R36">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7:R8">
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9:R9">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X7:X8">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X9">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X10:X13">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X9">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+  <conditionalFormatting sqref="B23:AJ23">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X10:X13">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+  <conditionalFormatting sqref="X23 P23:R23">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
more data and contracts
</commit_message>
<xml_diff>
--- a/assets/contracts and data.xlsx
+++ b/assets/contracts and data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\link-builder\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF1B08F-B50A-446C-84EB-333BF4AA30B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C91514-02DC-4B8C-ACDF-8B55AD656E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
   <si>
     <t>LinkPal</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Etherisc Flight Insurance</t>
+  </si>
+  <si>
+    <t>Twitter</t>
   </si>
 </sst>
 </file>
@@ -327,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -386,6 +389,19 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ68"/>
+  <dimension ref="A1:AR68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,39 +771,40 @@
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" style="21" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="29" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
@@ -803,104 +820,107 @@
       <c r="F1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-    </row>
-    <row r="2" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ1" s="1"/>
+    </row>
+    <row r="2" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>44</v>
       </c>
@@ -939,15 +959,16 @@
       <c r="AH2" s="18"/>
       <c r="AI2" s="18"/>
       <c r="AJ2" s="18"/>
-      <c r="AK2" s="22"/>
+      <c r="AK2" s="18"/>
       <c r="AL2" s="22"/>
       <c r="AM2" s="22"/>
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
       <c r="AP2" s="22"/>
-      <c r="AQ2" s="23"/>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="23"/>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>45</v>
       </c>
@@ -962,29 +983,29 @@
         <v>22</v>
       </c>
       <c r="F3" s="18"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="13"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="12"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="18"/>
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="18"/>
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="18"/>
       <c r="AD3" s="13"/>
       <c r="AE3" s="13"/>
       <c r="AF3" s="13"/>
@@ -992,15 +1013,16 @@
       <c r="AH3" s="13"/>
       <c r="AI3" s="13"/>
       <c r="AJ3" s="13"/>
-      <c r="AK3" s="14"/>
+      <c r="AK3" s="13"/>
       <c r="AL3" s="14"/>
       <c r="AM3" s="14"/>
       <c r="AN3" s="14"/>
       <c r="AO3" s="14"/>
       <c r="AP3" s="14"/>
-      <c r="AQ3" s="15"/>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ3" s="14"/>
+      <c r="AR3" s="15"/>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -1011,29 +1033,29 @@
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="12"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="18"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="18"/>
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
       <c r="AA4" s="13"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="18"/>
       <c r="AD4" s="13"/>
       <c r="AE4" s="13"/>
       <c r="AF4" s="13"/>
@@ -1041,15 +1063,16 @@
       <c r="AH4" s="13"/>
       <c r="AI4" s="13"/>
       <c r="AJ4" s="13"/>
-      <c r="AK4" s="14"/>
+      <c r="AK4" s="13"/>
       <c r="AL4" s="14"/>
       <c r="AM4" s="14"/>
       <c r="AN4" s="14"/>
       <c r="AO4" s="14"/>
       <c r="AP4" s="14"/>
-      <c r="AQ4" s="15"/>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ4" s="14"/>
+      <c r="AR4" s="15"/>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
@@ -1060,29 +1083,29 @@
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
       <c r="T5" s="13"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="18"/>
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
       <c r="AA5" s="13"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="18"/>
       <c r="AD5" s="13"/>
       <c r="AE5" s="13"/>
       <c r="AF5" s="13"/>
@@ -1090,15 +1113,16 @@
       <c r="AH5" s="13"/>
       <c r="AI5" s="13"/>
       <c r="AJ5" s="13"/>
-      <c r="AK5" s="14"/>
+      <c r="AK5" s="13"/>
       <c r="AL5" s="14"/>
       <c r="AM5" s="14"/>
       <c r="AN5" s="14"/>
       <c r="AO5" s="14"/>
       <c r="AP5" s="14"/>
-      <c r="AQ5" s="15"/>
-    </row>
-    <row r="6" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AQ5" s="14"/>
+      <c r="AR5" s="15"/>
+    </row>
+    <row r="6" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
@@ -1137,15 +1161,16 @@
       <c r="AH6" s="18"/>
       <c r="AI6" s="18"/>
       <c r="AJ6" s="18"/>
-      <c r="AK6" s="22"/>
+      <c r="AK6" s="18"/>
       <c r="AL6" s="22"/>
       <c r="AM6" s="22"/>
       <c r="AN6" s="22"/>
       <c r="AO6" s="22"/>
       <c r="AP6" s="22"/>
-      <c r="AQ6" s="23"/>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="22"/>
+      <c r="AR6" s="23"/>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>0</v>
       </c>
@@ -1156,39 +1181,39 @@
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="19"/>
-      <c r="G7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="17"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="19"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="19"/>
       <c r="Q7" s="17" t="s">
         <v>22</v>
       </c>
       <c r="R7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="U7" s="19"/>
-      <c r="V7" s="17"/>
+      <c r="S7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V7" s="19"/>
       <c r="W7" s="17"/>
       <c r="X7" s="17"/>
       <c r="Y7" s="17"/>
       <c r="Z7" s="17"/>
       <c r="AA7" s="17"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="19"/>
       <c r="AD7" s="17"/>
       <c r="AE7" s="17"/>
       <c r="AF7" s="17"/>
@@ -1196,15 +1221,16 @@
       <c r="AH7" s="17"/>
       <c r="AI7" s="17"/>
       <c r="AJ7" s="17"/>
-      <c r="AK7" s="15"/>
+      <c r="AK7" s="17"/>
       <c r="AL7" s="15"/>
       <c r="AM7" s="15"/>
       <c r="AN7" s="15"/>
       <c r="AO7" s="15"/>
       <c r="AP7" s="15"/>
       <c r="AQ7" s="15"/>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR7" s="15"/>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>21</v>
       </c>
@@ -1215,39 +1241,39 @@
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="17"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="19"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="O8" s="17"/>
+      <c r="P8" s="19"/>
       <c r="Q8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="R8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="U8" s="19"/>
-      <c r="V8" s="17"/>
+      <c r="S8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V8" s="19"/>
       <c r="W8" s="17"/>
       <c r="X8" s="17"/>
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
       <c r="AA8" s="17"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="19"/>
       <c r="AD8" s="17"/>
       <c r="AE8" s="17"/>
       <c r="AF8" s="17"/>
@@ -1255,15 +1281,16 @@
       <c r="AH8" s="17"/>
       <c r="AI8" s="17"/>
       <c r="AJ8" s="17"/>
-      <c r="AK8" s="15"/>
+      <c r="AK8" s="17"/>
       <c r="AL8" s="15"/>
       <c r="AM8" s="15"/>
       <c r="AN8" s="15"/>
       <c r="AO8" s="15"/>
       <c r="AP8" s="15"/>
       <c r="AQ8" s="15"/>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR8" s="15"/>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1272,33 +1299,33 @@
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="19"/>
-      <c r="G9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="17"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="19"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="19"/>
       <c r="W9" s="17"/>
       <c r="X9" s="17"/>
       <c r="Y9" s="17"/>
       <c r="Z9" s="17"/>
       <c r="AA9" s="17"/>
-      <c r="AB9" s="19"/>
-      <c r="AC9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="19"/>
       <c r="AD9" s="17"/>
       <c r="AE9" s="17"/>
       <c r="AF9" s="17"/>
@@ -1306,16 +1333,17 @@
       <c r="AH9" s="17"/>
       <c r="AI9" s="17"/>
       <c r="AJ9" s="17"/>
-      <c r="AK9" s="15"/>
+      <c r="AK9" s="17"/>
       <c r="AL9" s="15"/>
       <c r="AM9" s="15"/>
       <c r="AN9" s="15"/>
       <c r="AO9" s="15"/>
       <c r="AP9" s="15"/>
       <c r="AQ9" s="15"/>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="AR9" s="15"/>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="18"/>
@@ -1323,39 +1351,39 @@
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="O10" s="17"/>
+      <c r="P10" s="19"/>
       <c r="Q10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="R10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="U10" s="19"/>
-      <c r="V10" s="17"/>
+      <c r="S10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V10" s="19"/>
       <c r="W10" s="17"/>
       <c r="X10" s="17"/>
       <c r="Y10" s="17"/>
       <c r="Z10" s="17"/>
       <c r="AA10" s="17"/>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="17"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="19"/>
       <c r="AD10" s="17"/>
       <c r="AE10" s="17"/>
       <c r="AF10" s="17"/>
@@ -1363,15 +1391,16 @@
       <c r="AH10" s="17"/>
       <c r="AI10" s="17"/>
       <c r="AJ10" s="17"/>
-      <c r="AK10" s="15"/>
+      <c r="AK10" s="17"/>
       <c r="AL10" s="15"/>
       <c r="AM10" s="15"/>
       <c r="AN10" s="15"/>
       <c r="AO10" s="15"/>
       <c r="AP10" s="15"/>
       <c r="AQ10" s="15"/>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR10" s="15"/>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>52</v>
       </c>
@@ -1386,29 +1415,29 @@
         <v>22</v>
       </c>
       <c r="F11" s="19"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="19"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="19"/>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
       <c r="T11" s="17"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="19"/>
       <c r="W11" s="17"/>
       <c r="X11" s="17"/>
       <c r="Y11" s="17"/>
       <c r="Z11" s="17"/>
       <c r="AA11" s="17"/>
-      <c r="AB11" s="19"/>
-      <c r="AC11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="19"/>
       <c r="AD11" s="17"/>
       <c r="AE11" s="17"/>
       <c r="AF11" s="17"/>
@@ -1416,15 +1445,16 @@
       <c r="AH11" s="17"/>
       <c r="AI11" s="17"/>
       <c r="AJ11" s="17"/>
-      <c r="AK11" s="15"/>
+      <c r="AK11" s="17"/>
       <c r="AL11" s="15"/>
       <c r="AM11" s="15"/>
       <c r="AN11" s="15"/>
       <c r="AO11" s="15"/>
       <c r="AP11" s="15"/>
       <c r="AQ11" s="15"/>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR11" s="15"/>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>53</v>
       </c>
@@ -1435,37 +1465,37 @@
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="19"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="O12" s="17"/>
+      <c r="P12" s="19"/>
       <c r="Q12" s="17" t="s">
         <v>22</v>
       </c>
       <c r="R12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="U12" s="19"/>
-      <c r="V12" s="17"/>
+      <c r="S12" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V12" s="19"/>
       <c r="W12" s="17"/>
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
       <c r="Z12" s="17"/>
       <c r="AA12" s="17"/>
-      <c r="AB12" s="19"/>
-      <c r="AC12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="19"/>
       <c r="AD12" s="17"/>
       <c r="AE12" s="17"/>
       <c r="AF12" s="17"/>
@@ -1473,15 +1503,16 @@
       <c r="AH12" s="17"/>
       <c r="AI12" s="17"/>
       <c r="AJ12" s="17"/>
-      <c r="AK12" s="15"/>
+      <c r="AK12" s="17"/>
       <c r="AL12" s="15"/>
       <c r="AM12" s="15"/>
       <c r="AN12" s="15"/>
       <c r="AO12" s="15"/>
       <c r="AP12" s="15"/>
       <c r="AQ12" s="15"/>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR12" s="15"/>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>68</v>
       </c>
@@ -1490,33 +1521,33 @@
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="19"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
-      <c r="M13" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="M13" s="17"/>
       <c r="N13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="19"/>
-      <c r="P13" s="17"/>
+      <c r="O13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" s="19"/>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="19"/>
       <c r="W13" s="17"/>
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
       <c r="Z13" s="17"/>
       <c r="AA13" s="17"/>
-      <c r="AB13" s="19"/>
-      <c r="AC13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="19"/>
       <c r="AD13" s="17"/>
       <c r="AE13" s="17"/>
       <c r="AF13" s="17"/>
@@ -1524,15 +1555,16 @@
       <c r="AH13" s="17"/>
       <c r="AI13" s="17"/>
       <c r="AJ13" s="17"/>
-      <c r="AK13" s="15"/>
+      <c r="AK13" s="17"/>
       <c r="AL13" s="15"/>
       <c r="AM13" s="15"/>
       <c r="AN13" s="15"/>
       <c r="AO13" s="15"/>
       <c r="AP13" s="15"/>
       <c r="AQ13" s="15"/>
-    </row>
-    <row r="14" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AR13" s="15"/>
+    </row>
+    <row r="14" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1571,15 +1603,16 @@
       <c r="AH14" s="18"/>
       <c r="AI14" s="18"/>
       <c r="AJ14" s="18"/>
-      <c r="AK14" s="22"/>
+      <c r="AK14" s="18"/>
       <c r="AL14" s="22"/>
       <c r="AM14" s="22"/>
       <c r="AN14" s="22"/>
       <c r="AO14" s="22"/>
       <c r="AP14" s="22"/>
-      <c r="AQ14" s="23"/>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ14" s="22"/>
+      <c r="AR14" s="23"/>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>59</v>
       </c>
@@ -1594,29 +1627,29 @@
         <v>22</v>
       </c>
       <c r="F15" s="18"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="12"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="18"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="18"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="18"/>
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
       <c r="AA15" s="13"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="18"/>
       <c r="AD15" s="13"/>
       <c r="AE15" s="13"/>
       <c r="AF15" s="13"/>
@@ -1624,15 +1657,16 @@
       <c r="AH15" s="13"/>
       <c r="AI15" s="13"/>
       <c r="AJ15" s="13"/>
-      <c r="AK15" s="14"/>
+      <c r="AK15" s="13"/>
       <c r="AL15" s="14"/>
       <c r="AM15" s="14"/>
       <c r="AN15" s="14"/>
       <c r="AO15" s="14"/>
       <c r="AP15" s="14"/>
-      <c r="AQ15" s="15"/>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ15" s="14"/>
+      <c r="AR15" s="15"/>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>43</v>
       </c>
@@ -1647,29 +1681,29 @@
         <v>22</v>
       </c>
       <c r="F16" s="19"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="17"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="19"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="19"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
       <c r="S16" s="17"/>
       <c r="T16" s="17"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="19"/>
       <c r="W16" s="17"/>
       <c r="X16" s="17"/>
       <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
       <c r="AA16" s="17"/>
-      <c r="AB16" s="19"/>
-      <c r="AC16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="19"/>
       <c r="AD16" s="17"/>
       <c r="AE16" s="17"/>
       <c r="AF16" s="17"/>
@@ -1677,15 +1711,16 @@
       <c r="AH16" s="17"/>
       <c r="AI16" s="17"/>
       <c r="AJ16" s="17"/>
-      <c r="AK16" s="15"/>
+      <c r="AK16" s="17"/>
       <c r="AL16" s="15"/>
       <c r="AM16" s="15"/>
       <c r="AN16" s="15"/>
       <c r="AO16" s="15"/>
       <c r="AP16" s="15"/>
       <c r="AQ16" s="15"/>
-    </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR16" s="15"/>
+    </row>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1700,29 +1735,29 @@
         <v>22</v>
       </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="19"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="19"/>
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="19"/>
       <c r="W17" s="17"/>
       <c r="X17" s="17"/>
       <c r="Y17" s="17"/>
       <c r="Z17" s="17"/>
       <c r="AA17" s="17"/>
-      <c r="AB17" s="19"/>
-      <c r="AC17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="19"/>
       <c r="AD17" s="17"/>
       <c r="AE17" s="17"/>
       <c r="AF17" s="17"/>
@@ -1730,15 +1765,16 @@
       <c r="AH17" s="17"/>
       <c r="AI17" s="17"/>
       <c r="AJ17" s="17"/>
-      <c r="AK17" s="15"/>
+      <c r="AK17" s="17"/>
       <c r="AL17" s="15"/>
       <c r="AM17" s="15"/>
       <c r="AN17" s="15"/>
       <c r="AO17" s="15"/>
       <c r="AP17" s="15"/>
       <c r="AQ17" s="15"/>
-    </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR17" s="15"/>
+    </row>
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>39</v>
       </c>
@@ -1753,29 +1789,29 @@
         <v>22</v>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="19"/>
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="19"/>
       <c r="Q18" s="17"/>
       <c r="R18" s="17"/>
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="19"/>
       <c r="W18" s="17"/>
       <c r="X18" s="17"/>
       <c r="Y18" s="17"/>
       <c r="Z18" s="17"/>
       <c r="AA18" s="17"/>
-      <c r="AB18" s="19"/>
-      <c r="AC18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="19"/>
       <c r="AD18" s="17"/>
       <c r="AE18" s="17"/>
       <c r="AF18" s="17"/>
@@ -1783,15 +1819,16 @@
       <c r="AH18" s="17"/>
       <c r="AI18" s="17"/>
       <c r="AJ18" s="17"/>
-      <c r="AK18" s="15"/>
+      <c r="AK18" s="17"/>
       <c r="AL18" s="15"/>
       <c r="AM18" s="15"/>
       <c r="AN18" s="15"/>
       <c r="AO18" s="15"/>
       <c r="AP18" s="15"/>
       <c r="AQ18" s="15"/>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR18" s="15"/>
+    </row>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>40</v>
       </c>
@@ -1806,29 +1843,29 @@
         <v>22</v>
       </c>
       <c r="F19" s="19"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="19"/>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="19"/>
       <c r="Q19" s="17"/>
       <c r="R19" s="17"/>
       <c r="S19" s="17"/>
       <c r="T19" s="17"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="19"/>
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
       <c r="Y19" s="17"/>
       <c r="Z19" s="17"/>
       <c r="AA19" s="17"/>
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="19"/>
       <c r="AD19" s="17"/>
       <c r="AE19" s="17"/>
       <c r="AF19" s="17"/>
@@ -1836,15 +1873,16 @@
       <c r="AH19" s="17"/>
       <c r="AI19" s="17"/>
       <c r="AJ19" s="17"/>
-      <c r="AK19" s="15"/>
+      <c r="AK19" s="17"/>
       <c r="AL19" s="15"/>
       <c r="AM19" s="15"/>
       <c r="AN19" s="15"/>
       <c r="AO19" s="15"/>
       <c r="AP19" s="15"/>
       <c r="AQ19" s="15"/>
-    </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR19" s="15"/>
+    </row>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1859,29 +1897,29 @@
         <v>22</v>
       </c>
       <c r="F20" s="19"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="19"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="19"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
       <c r="T20" s="17"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="19"/>
       <c r="W20" s="17"/>
       <c r="X20" s="17"/>
       <c r="Y20" s="17"/>
       <c r="Z20" s="17"/>
       <c r="AA20" s="17"/>
-      <c r="AB20" s="19"/>
-      <c r="AC20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="19"/>
       <c r="AD20" s="17"/>
       <c r="AE20" s="17"/>
       <c r="AF20" s="17"/>
@@ -1889,15 +1927,16 @@
       <c r="AH20" s="17"/>
       <c r="AI20" s="17"/>
       <c r="AJ20" s="17"/>
-      <c r="AK20" s="15"/>
+      <c r="AK20" s="17"/>
       <c r="AL20" s="15"/>
       <c r="AM20" s="15"/>
       <c r="AN20" s="15"/>
       <c r="AO20" s="15"/>
       <c r="AP20" s="15"/>
       <c r="AQ20" s="15"/>
-    </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR20" s="15"/>
+    </row>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1912,33 +1951,33 @@
         <v>22</v>
       </c>
       <c r="F21" s="19"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="19"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="19"/>
       <c r="Q21" s="17"/>
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
-      <c r="T21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="U21" s="19"/>
-      <c r="V21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V21" s="19"/>
       <c r="W21" s="17"/>
       <c r="X21" s="17"/>
-      <c r="Y21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AA21" s="17"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="17"/>
+      <c r="AB21" s="17"/>
+      <c r="AC21" s="19"/>
       <c r="AD21" s="17"/>
       <c r="AE21" s="17"/>
       <c r="AF21" s="17"/>
@@ -1946,15 +1985,16 @@
       <c r="AH21" s="17"/>
       <c r="AI21" s="17"/>
       <c r="AJ21" s="17"/>
-      <c r="AK21" s="15"/>
+      <c r="AK21" s="17"/>
       <c r="AL21" s="15"/>
       <c r="AM21" s="15"/>
       <c r="AN21" s="15"/>
       <c r="AO21" s="15"/>
       <c r="AP21" s="15"/>
       <c r="AQ21" s="15"/>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR21" s="15"/>
+    </row>
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>69</v>
       </c>
@@ -1969,37 +2009,37 @@
         <v>22</v>
       </c>
       <c r="F22" s="19"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="17"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="19"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="L22" s="17"/>
       <c r="M22" s="17" t="s">
         <v>22</v>
       </c>
       <c r="N22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="19"/>
-      <c r="P22" s="17"/>
+      <c r="O22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" s="19"/>
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
       <c r="T22" s="17"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="19"/>
       <c r="W22" s="17"/>
       <c r="X22" s="17"/>
       <c r="Y22" s="17"/>
-      <c r="Z22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA22" s="17"/>
-      <c r="AB22" s="19"/>
-      <c r="AC22" s="17"/>
+      <c r="Z22" s="17"/>
+      <c r="AA22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB22" s="17"/>
+      <c r="AC22" s="19"/>
       <c r="AD22" s="17"/>
       <c r="AE22" s="17"/>
       <c r="AF22" s="17"/>
@@ -2007,15 +2047,16 @@
       <c r="AH22" s="17"/>
       <c r="AI22" s="17"/>
       <c r="AJ22" s="17"/>
-      <c r="AK22" s="15"/>
+      <c r="AK22" s="17"/>
       <c r="AL22" s="15"/>
       <c r="AM22" s="15"/>
       <c r="AN22" s="15"/>
       <c r="AO22" s="15"/>
       <c r="AP22" s="15"/>
       <c r="AQ22" s="15"/>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR22" s="15"/>
+    </row>
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>5</v>
       </c>
@@ -2024,51 +2065,52 @@
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="17"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="19"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N23" s="17"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="19"/>
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
-      <c r="S23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T23" s="17"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U23" s="17"/>
+      <c r="V23" s="19"/>
       <c r="W23" s="17"/>
       <c r="X23" s="17"/>
       <c r="Y23" s="17"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="17"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD23" s="17"/>
+      <c r="AB23" s="17"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AE23" s="17"/>
       <c r="AF23" s="17"/>
       <c r="AG23" s="17"/>
       <c r="AH23" s="17"/>
       <c r="AI23" s="17"/>
       <c r="AJ23" s="17"/>
-      <c r="AK23" s="15"/>
+      <c r="AK23" s="17"/>
       <c r="AL23" s="15"/>
       <c r="AM23" s="15"/>
       <c r="AN23" s="15"/>
       <c r="AO23" s="15"/>
       <c r="AP23" s="15"/>
       <c r="AQ23" s="15"/>
-    </row>
-    <row r="24" spans="1:43" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AR23" s="15"/>
+    </row>
+    <row r="24" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>36</v>
       </c>
@@ -2107,15 +2149,16 @@
       <c r="AH24" s="19"/>
       <c r="AI24" s="19"/>
       <c r="AJ24" s="19"/>
-      <c r="AK24" s="23"/>
+      <c r="AK24" s="19"/>
       <c r="AL24" s="23"/>
       <c r="AM24" s="23"/>
       <c r="AN24" s="23"/>
       <c r="AO24" s="23"/>
       <c r="AP24" s="23"/>
       <c r="AQ24" s="23"/>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR24" s="23"/>
+    </row>
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>1</v>
       </c>
@@ -2124,35 +2167,35 @@
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="19"/>
-      <c r="G25" s="17"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="17"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="19"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N25" s="17"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="19"/>
       <c r="Q25" s="17"/>
       <c r="R25" s="17"/>
-      <c r="S25" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T25" s="17"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U25" s="17"/>
+      <c r="V25" s="19"/>
       <c r="W25" s="17"/>
-      <c r="X25" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="Z25" s="17"/>
       <c r="AA25" s="17"/>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="17"/>
+      <c r="AB25" s="17"/>
+      <c r="AC25" s="19"/>
       <c r="AD25" s="17"/>
       <c r="AE25" s="17"/>
       <c r="AF25" s="17"/>
@@ -2160,15 +2203,16 @@
       <c r="AH25" s="17"/>
       <c r="AI25" s="17"/>
       <c r="AJ25" s="17"/>
-      <c r="AK25" s="15"/>
+      <c r="AK25" s="17"/>
       <c r="AL25" s="15"/>
       <c r="AM25" s="15"/>
       <c r="AN25" s="15"/>
       <c r="AO25" s="15"/>
       <c r="AP25" s="15"/>
       <c r="AQ25" s="15"/>
-    </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR25" s="15"/>
+    </row>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>2</v>
       </c>
@@ -2177,51 +2221,52 @@
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="17"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="17"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="19"/>
       <c r="K26" s="17"/>
-      <c r="L26" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N26" s="17"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="19"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
-      <c r="S26" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T26" s="17"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26" s="17"/>
+      <c r="V26" s="19"/>
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
       <c r="Y26" s="17"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="17"/>
-      <c r="AB26" s="19"/>
-      <c r="AC26" s="17"/>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="19"/>
       <c r="AD26" s="17"/>
       <c r="AE26" s="17"/>
-      <c r="AF26" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG26" s="17"/>
+      <c r="AF26" s="17"/>
+      <c r="AG26" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AH26" s="17"/>
       <c r="AI26" s="17"/>
       <c r="AJ26" s="17"/>
-      <c r="AK26" s="15"/>
+      <c r="AK26" s="17"/>
       <c r="AL26" s="15"/>
       <c r="AM26" s="15"/>
       <c r="AN26" s="15"/>
       <c r="AO26" s="15"/>
       <c r="AP26" s="15"/>
       <c r="AQ26" s="15"/>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR26" s="15"/>
+    </row>
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>50</v>
       </c>
@@ -2230,35 +2275,35 @@
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="17"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="19"/>
       <c r="K27" s="17"/>
-      <c r="L27" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N27" s="17"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="19"/>
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
-      <c r="S27" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T27" s="17"/>
-      <c r="U27" s="19"/>
-      <c r="V27" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="W27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U27" s="17"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="X27" s="17"/>
       <c r="Y27" s="17"/>
       <c r="Z27" s="17"/>
       <c r="AA27" s="17"/>
-      <c r="AB27" s="19"/>
-      <c r="AC27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="19"/>
       <c r="AD27" s="17"/>
       <c r="AE27" s="17"/>
       <c r="AF27" s="17"/>
@@ -2266,15 +2311,16 @@
       <c r="AH27" s="17"/>
       <c r="AI27" s="17"/>
       <c r="AJ27" s="17"/>
-      <c r="AK27" s="15"/>
+      <c r="AK27" s="17"/>
       <c r="AL27" s="15"/>
       <c r="AM27" s="15"/>
       <c r="AN27" s="15"/>
       <c r="AO27" s="15"/>
       <c r="AP27" s="15"/>
       <c r="AQ27" s="15"/>
-    </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR27" s="15"/>
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>3</v>
       </c>
@@ -2283,51 +2329,52 @@
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="27"/>
       <c r="H28" s="17"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="19"/>
       <c r="K28" s="17"/>
-      <c r="L28" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N28" s="17"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="19"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
-      <c r="S28" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T28" s="17"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" s="17"/>
+      <c r="V28" s="19"/>
       <c r="W28" s="17"/>
       <c r="X28" s="17"/>
       <c r="Y28" s="17"/>
       <c r="Z28" s="17"/>
       <c r="AA28" s="17"/>
-      <c r="AB28" s="19"/>
-      <c r="AC28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="19"/>
       <c r="AD28" s="17"/>
       <c r="AE28" s="17"/>
       <c r="AF28" s="17"/>
       <c r="AG28" s="17"/>
       <c r="AH28" s="17"/>
-      <c r="AI28" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ28" s="17"/>
-      <c r="AK28" s="15"/>
+      <c r="AI28" s="17"/>
+      <c r="AJ28" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK28" s="17"/>
       <c r="AL28" s="15"/>
       <c r="AM28" s="15"/>
       <c r="AN28" s="15"/>
       <c r="AO28" s="15"/>
       <c r="AP28" s="15"/>
       <c r="AQ28" s="15"/>
-    </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR28" s="15"/>
+    </row>
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -2336,35 +2383,35 @@
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="17"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="19"/>
       <c r="K29" s="17"/>
-      <c r="L29" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N29" s="17"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="19"/>
       <c r="Q29" s="17"/>
       <c r="R29" s="17"/>
-      <c r="S29" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T29" s="17"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U29" s="17"/>
+      <c r="V29" s="19"/>
       <c r="W29" s="17"/>
       <c r="X29" s="17"/>
       <c r="Y29" s="17"/>
       <c r="Z29" s="17"/>
-      <c r="AA29" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB29" s="19"/>
-      <c r="AC29" s="17"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC29" s="19"/>
       <c r="AD29" s="17"/>
       <c r="AE29" s="17"/>
       <c r="AF29" s="17"/>
@@ -2372,15 +2419,16 @@
       <c r="AH29" s="17"/>
       <c r="AI29" s="17"/>
       <c r="AJ29" s="17"/>
-      <c r="AK29" s="15"/>
+      <c r="AK29" s="17"/>
       <c r="AL29" s="15"/>
       <c r="AM29" s="15"/>
       <c r="AN29" s="15"/>
       <c r="AO29" s="15"/>
       <c r="AP29" s="15"/>
       <c r="AQ29" s="15"/>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR29" s="15"/>
+    </row>
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -2389,51 +2437,52 @@
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="19"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="27"/>
       <c r="H30" s="17"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="19"/>
       <c r="K30" s="17"/>
-      <c r="L30" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N30" s="17"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="19"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="17"/>
-      <c r="S30" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T30" s="17"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U30" s="17"/>
+      <c r="V30" s="19"/>
       <c r="W30" s="17"/>
       <c r="X30" s="17"/>
       <c r="Y30" s="17"/>
       <c r="Z30" s="17"/>
       <c r="AA30" s="17"/>
-      <c r="AB30" s="19"/>
-      <c r="AC30" s="17"/>
-      <c r="AD30" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE30" s="17"/>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="17"/>
+      <c r="AE30" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AF30" s="17"/>
       <c r="AG30" s="17"/>
       <c r="AH30" s="17"/>
       <c r="AI30" s="17"/>
       <c r="AJ30" s="17"/>
-      <c r="AK30" s="15"/>
+      <c r="AK30" s="17"/>
       <c r="AL30" s="15"/>
       <c r="AM30" s="15"/>
       <c r="AN30" s="15"/>
       <c r="AO30" s="15"/>
       <c r="AP30" s="15"/>
       <c r="AQ30" s="15"/>
-    </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR30" s="15"/>
+    </row>
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -2442,51 +2491,52 @@
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="17"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="19"/>
       <c r="K31" s="17"/>
-      <c r="L31" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N31" s="17"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="19"/>
       <c r="Q31" s="17"/>
       <c r="R31" s="17"/>
-      <c r="S31" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T31" s="17"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U31" s="17"/>
+      <c r="V31" s="19"/>
       <c r="W31" s="17"/>
       <c r="X31" s="17"/>
       <c r="Y31" s="17"/>
       <c r="Z31" s="17"/>
       <c r="AA31" s="17"/>
-      <c r="AB31" s="19"/>
-      <c r="AC31" s="17"/>
+      <c r="AB31" s="17"/>
+      <c r="AC31" s="19"/>
       <c r="AD31" s="17"/>
-      <c r="AE31" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF31" s="17"/>
+      <c r="AE31" s="17"/>
+      <c r="AF31" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AG31" s="17"/>
       <c r="AH31" s="17"/>
       <c r="AI31" s="17"/>
       <c r="AJ31" s="17"/>
-      <c r="AK31" s="15"/>
+      <c r="AK31" s="17"/>
       <c r="AL31" s="15"/>
       <c r="AM31" s="15"/>
       <c r="AN31" s="15"/>
       <c r="AO31" s="15"/>
       <c r="AP31" s="15"/>
       <c r="AQ31" s="15"/>
-    </row>
-    <row r="32" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR31" s="15"/>
+    </row>
+    <row r="32" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
@@ -2495,49 +2545,50 @@
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
       <c r="F32" s="19"/>
-      <c r="G32" s="17"/>
+      <c r="G32" s="27"/>
       <c r="H32" s="17"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="19"/>
       <c r="K32" s="17"/>
-      <c r="L32" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N32" s="17"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="19"/>
       <c r="Q32" s="17"/>
       <c r="R32" s="17"/>
       <c r="S32" s="17"/>
       <c r="T32" s="17"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="19"/>
       <c r="W32" s="17"/>
       <c r="X32" s="17"/>
       <c r="Y32" s="17"/>
       <c r="Z32" s="17"/>
       <c r="AA32" s="17"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="17"/>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="19"/>
       <c r="AD32" s="17"/>
       <c r="AE32" s="17"/>
       <c r="AF32" s="17"/>
       <c r="AG32" s="17"/>
       <c r="AH32" s="17"/>
       <c r="AI32" s="17"/>
-      <c r="AJ32" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK32" s="15"/>
+      <c r="AJ32" s="17"/>
+      <c r="AK32" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AL32" s="15"/>
       <c r="AM32" s="15"/>
       <c r="AN32" s="15"/>
       <c r="AO32" s="15"/>
       <c r="AP32" s="15"/>
       <c r="AQ32" s="15"/>
-    </row>
-    <row r="33" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR32" s="15"/>
+    </row>
+    <row r="33" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
@@ -2546,33 +2597,33 @@
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
       <c r="F33" s="19"/>
-      <c r="G33" s="17"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="17"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="19"/>
       <c r="K33" s="17"/>
-      <c r="L33" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N33" s="17"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="19"/>
       <c r="Q33" s="17"/>
       <c r="R33" s="17"/>
-      <c r="S33" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T33" s="17"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U33" s="17"/>
+      <c r="V33" s="19"/>
       <c r="W33" s="17"/>
       <c r="X33" s="17"/>
       <c r="Y33" s="17"/>
       <c r="Z33" s="17"/>
       <c r="AA33" s="17"/>
-      <c r="AB33" s="19"/>
-      <c r="AC33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="19"/>
       <c r="AD33" s="17"/>
       <c r="AE33" s="17"/>
       <c r="AF33" s="17"/>
@@ -2580,15 +2631,16 @@
       <c r="AH33" s="17"/>
       <c r="AI33" s="17"/>
       <c r="AJ33" s="17"/>
-      <c r="AK33" s="15"/>
+      <c r="AK33" s="17"/>
       <c r="AL33" s="15"/>
       <c r="AM33" s="15"/>
       <c r="AN33" s="15"/>
       <c r="AO33" s="15"/>
       <c r="AP33" s="15"/>
       <c r="AQ33" s="15"/>
-    </row>
-    <row r="34" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR33" s="15"/>
+    </row>
+    <row r="34" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>19</v>
       </c>
@@ -2597,29 +2649,29 @@
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="17"/>
+      <c r="G34" s="27"/>
       <c r="H34" s="17"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="19"/>
       <c r="K34" s="17"/>
       <c r="L34" s="17"/>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="19"/>
       <c r="Q34" s="17"/>
       <c r="R34" s="17"/>
       <c r="S34" s="17"/>
       <c r="T34" s="17"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="19"/>
       <c r="W34" s="17"/>
       <c r="X34" s="17"/>
       <c r="Y34" s="17"/>
       <c r="Z34" s="17"/>
       <c r="AA34" s="17"/>
-      <c r="AB34" s="19"/>
-      <c r="AC34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="19"/>
       <c r="AD34" s="17"/>
       <c r="AE34" s="17"/>
       <c r="AF34" s="17"/>
@@ -2627,15 +2679,16 @@
       <c r="AH34" s="17"/>
       <c r="AI34" s="17"/>
       <c r="AJ34" s="17"/>
-      <c r="AK34" s="15"/>
+      <c r="AK34" s="17"/>
       <c r="AL34" s="15"/>
       <c r="AM34" s="15"/>
       <c r="AN34" s="15"/>
       <c r="AO34" s="15"/>
       <c r="AP34" s="15"/>
       <c r="AQ34" s="15"/>
-    </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR34" s="15"/>
+    </row>
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -2644,31 +2697,31 @@
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="17"/>
+      <c r="G35" s="27"/>
       <c r="H35" s="17"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="19"/>
       <c r="K35" s="17"/>
-      <c r="L35" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="N35" s="17"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="19"/>
       <c r="Q35" s="17"/>
       <c r="R35" s="17"/>
       <c r="S35" s="17"/>
       <c r="T35" s="17"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="19"/>
       <c r="W35" s="17"/>
       <c r="X35" s="17"/>
       <c r="Y35" s="17"/>
       <c r="Z35" s="17"/>
       <c r="AA35" s="17"/>
-      <c r="AB35" s="19"/>
-      <c r="AC35" s="17"/>
+      <c r="AB35" s="17"/>
+      <c r="AC35" s="19"/>
       <c r="AD35" s="17"/>
       <c r="AE35" s="17"/>
       <c r="AF35" s="17"/>
@@ -2676,44 +2729,45 @@
       <c r="AH35" s="17"/>
       <c r="AI35" s="17"/>
       <c r="AJ35" s="17"/>
-      <c r="AK35" s="15"/>
+      <c r="AK35" s="17"/>
       <c r="AL35" s="15"/>
       <c r="AM35" s="15"/>
       <c r="AN35" s="15"/>
       <c r="AO35" s="15"/>
       <c r="AP35" s="15"/>
       <c r="AQ35" s="15"/>
-    </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR35" s="15"/>
+    </row>
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="18"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
       <c r="F36" s="19"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="27"/>
       <c r="H36" s="17"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="19"/>
       <c r="K36" s="17"/>
       <c r="L36" s="17"/>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="19"/>
       <c r="Q36" s="17"/>
       <c r="R36" s="17"/>
       <c r="S36" s="17"/>
       <c r="T36" s="17"/>
-      <c r="U36" s="19"/>
-      <c r="V36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="19"/>
       <c r="W36" s="17"/>
       <c r="X36" s="17"/>
       <c r="Y36" s="17"/>
       <c r="Z36" s="17"/>
       <c r="AA36" s="17"/>
-      <c r="AB36" s="19"/>
-      <c r="AC36" s="17"/>
+      <c r="AB36" s="17"/>
+      <c r="AC36" s="19"/>
       <c r="AD36" s="17"/>
       <c r="AE36" s="17"/>
       <c r="AF36" s="17"/>
@@ -2721,43 +2775,44 @@
       <c r="AH36" s="17"/>
       <c r="AI36" s="17"/>
       <c r="AJ36" s="17"/>
-      <c r="AK36" s="15"/>
+      <c r="AK36" s="17"/>
       <c r="AL36" s="15"/>
       <c r="AM36" s="15"/>
       <c r="AN36" s="15"/>
       <c r="AO36" s="15"/>
       <c r="AP36" s="15"/>
       <c r="AQ36" s="15"/>
-    </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR36" s="15"/>
+    </row>
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B37" s="19"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
       <c r="F37" s="19"/>
-      <c r="G37" s="17"/>
+      <c r="G37" s="27"/>
       <c r="H37" s="17"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="19"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="19"/>
       <c r="Q37" s="17"/>
       <c r="R37" s="17"/>
       <c r="S37" s="17"/>
       <c r="T37" s="17"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="19"/>
       <c r="W37" s="17"/>
       <c r="X37" s="17"/>
       <c r="Y37" s="17"/>
       <c r="Z37" s="17"/>
       <c r="AA37" s="17"/>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="17"/>
+      <c r="AB37" s="17"/>
+      <c r="AC37" s="19"/>
       <c r="AD37" s="17"/>
       <c r="AE37" s="17"/>
       <c r="AF37" s="17"/>
@@ -2765,43 +2820,44 @@
       <c r="AH37" s="17"/>
       <c r="AI37" s="17"/>
       <c r="AJ37" s="17"/>
-      <c r="AK37" s="15"/>
+      <c r="AK37" s="17"/>
       <c r="AL37" s="15"/>
       <c r="AM37" s="15"/>
       <c r="AN37" s="15"/>
       <c r="AO37" s="15"/>
       <c r="AP37" s="15"/>
       <c r="AQ37" s="15"/>
-    </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR37" s="15"/>
+    </row>
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B38" s="19"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="19"/>
-      <c r="G38" s="17"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="17"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="19"/>
       <c r="K38" s="17"/>
       <c r="L38" s="17"/>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="19"/>
       <c r="Q38" s="17"/>
       <c r="R38" s="17"/>
       <c r="S38" s="17"/>
       <c r="T38" s="17"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="19"/>
       <c r="W38" s="17"/>
       <c r="X38" s="17"/>
       <c r="Y38" s="17"/>
       <c r="Z38" s="17"/>
       <c r="AA38" s="17"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="17"/>
+      <c r="AB38" s="17"/>
+      <c r="AC38" s="19"/>
       <c r="AD38" s="17"/>
       <c r="AE38" s="17"/>
       <c r="AF38" s="17"/>
@@ -2809,43 +2865,44 @@
       <c r="AH38" s="17"/>
       <c r="AI38" s="17"/>
       <c r="AJ38" s="17"/>
-      <c r="AK38" s="15"/>
+      <c r="AK38" s="17"/>
       <c r="AL38" s="15"/>
       <c r="AM38" s="15"/>
       <c r="AN38" s="15"/>
       <c r="AO38" s="15"/>
       <c r="AP38" s="15"/>
       <c r="AQ38" s="15"/>
-    </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR38" s="15"/>
+    </row>
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B39" s="19"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
       <c r="F39" s="19"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="17"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="19"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="19"/>
       <c r="Q39" s="17"/>
       <c r="R39" s="17"/>
       <c r="S39" s="17"/>
       <c r="T39" s="17"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="19"/>
       <c r="W39" s="17"/>
       <c r="X39" s="17"/>
       <c r="Y39" s="17"/>
       <c r="Z39" s="17"/>
       <c r="AA39" s="17"/>
-      <c r="AB39" s="19"/>
-      <c r="AC39" s="17"/>
+      <c r="AB39" s="17"/>
+      <c r="AC39" s="19"/>
       <c r="AD39" s="17"/>
       <c r="AE39" s="17"/>
       <c r="AF39" s="17"/>
@@ -2853,43 +2910,44 @@
       <c r="AH39" s="17"/>
       <c r="AI39" s="17"/>
       <c r="AJ39" s="17"/>
-      <c r="AK39" s="15"/>
+      <c r="AK39" s="17"/>
       <c r="AL39" s="15"/>
       <c r="AM39" s="15"/>
       <c r="AN39" s="15"/>
       <c r="AO39" s="15"/>
       <c r="AP39" s="15"/>
       <c r="AQ39" s="15"/>
-    </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR39" s="15"/>
+    </row>
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B40" s="19"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
       <c r="F40" s="19"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="27"/>
       <c r="H40" s="17"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="19"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="19"/>
       <c r="Q40" s="17"/>
       <c r="R40" s="17"/>
       <c r="S40" s="17"/>
       <c r="T40" s="17"/>
-      <c r="U40" s="19"/>
-      <c r="V40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="19"/>
       <c r="W40" s="17"/>
       <c r="X40" s="17"/>
       <c r="Y40" s="17"/>
       <c r="Z40" s="17"/>
       <c r="AA40" s="17"/>
-      <c r="AB40" s="19"/>
-      <c r="AC40" s="17"/>
+      <c r="AB40" s="17"/>
+      <c r="AC40" s="19"/>
       <c r="AD40" s="17"/>
       <c r="AE40" s="17"/>
       <c r="AF40" s="17"/>
@@ -2897,43 +2955,44 @@
       <c r="AH40" s="17"/>
       <c r="AI40" s="17"/>
       <c r="AJ40" s="17"/>
-      <c r="AK40" s="15"/>
+      <c r="AK40" s="17"/>
       <c r="AL40" s="15"/>
       <c r="AM40" s="15"/>
       <c r="AN40" s="15"/>
       <c r="AO40" s="15"/>
       <c r="AP40" s="15"/>
       <c r="AQ40" s="15"/>
-    </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR40" s="15"/>
+    </row>
+    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B41" s="19"/>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
       <c r="F41" s="19"/>
-      <c r="G41" s="17"/>
+      <c r="G41" s="27"/>
       <c r="H41" s="17"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="19"/>
       <c r="K41" s="17"/>
       <c r="L41" s="17"/>
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="19"/>
       <c r="Q41" s="17"/>
       <c r="R41" s="17"/>
       <c r="S41" s="17"/>
       <c r="T41" s="17"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="17"/>
+      <c r="U41" s="17"/>
+      <c r="V41" s="19"/>
       <c r="W41" s="17"/>
       <c r="X41" s="17"/>
       <c r="Y41" s="17"/>
       <c r="Z41" s="17"/>
       <c r="AA41" s="17"/>
-      <c r="AB41" s="19"/>
-      <c r="AC41" s="17"/>
+      <c r="AB41" s="17"/>
+      <c r="AC41" s="19"/>
       <c r="AD41" s="17"/>
       <c r="AE41" s="17"/>
       <c r="AF41" s="17"/>
@@ -2941,43 +3000,44 @@
       <c r="AH41" s="17"/>
       <c r="AI41" s="17"/>
       <c r="AJ41" s="17"/>
-      <c r="AK41" s="15"/>
+      <c r="AK41" s="17"/>
       <c r="AL41" s="15"/>
       <c r="AM41" s="15"/>
       <c r="AN41" s="15"/>
       <c r="AO41" s="15"/>
       <c r="AP41" s="15"/>
       <c r="AQ41" s="15"/>
-    </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR41" s="15"/>
+    </row>
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B42" s="19"/>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
       <c r="F42" s="19"/>
-      <c r="G42" s="17"/>
+      <c r="G42" s="27"/>
       <c r="H42" s="17"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="19"/>
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="19"/>
       <c r="Q42" s="17"/>
       <c r="R42" s="17"/>
       <c r="S42" s="17"/>
       <c r="T42" s="17"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="19"/>
       <c r="W42" s="17"/>
       <c r="X42" s="17"/>
       <c r="Y42" s="17"/>
       <c r="Z42" s="17"/>
       <c r="AA42" s="17"/>
-      <c r="AB42" s="19"/>
-      <c r="AC42" s="17"/>
+      <c r="AB42" s="17"/>
+      <c r="AC42" s="19"/>
       <c r="AD42" s="17"/>
       <c r="AE42" s="17"/>
       <c r="AF42" s="17"/>
@@ -2985,43 +3045,44 @@
       <c r="AH42" s="17"/>
       <c r="AI42" s="17"/>
       <c r="AJ42" s="17"/>
-      <c r="AK42" s="15"/>
+      <c r="AK42" s="17"/>
       <c r="AL42" s="15"/>
       <c r="AM42" s="15"/>
       <c r="AN42" s="15"/>
       <c r="AO42" s="15"/>
       <c r="AP42" s="15"/>
       <c r="AQ42" s="15"/>
-    </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR42" s="15"/>
+    </row>
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B43" s="19"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
       <c r="F43" s="19"/>
-      <c r="G43" s="17"/>
+      <c r="G43" s="27"/>
       <c r="H43" s="17"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="19"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="19"/>
       <c r="Q43" s="17"/>
       <c r="R43" s="17"/>
       <c r="S43" s="17"/>
       <c r="T43" s="17"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="17"/>
+      <c r="U43" s="17"/>
+      <c r="V43" s="19"/>
       <c r="W43" s="17"/>
       <c r="X43" s="17"/>
       <c r="Y43" s="17"/>
       <c r="Z43" s="17"/>
       <c r="AA43" s="17"/>
-      <c r="AB43" s="19"/>
-      <c r="AC43" s="17"/>
+      <c r="AB43" s="17"/>
+      <c r="AC43" s="19"/>
       <c r="AD43" s="17"/>
       <c r="AE43" s="17"/>
       <c r="AF43" s="17"/>
@@ -3029,43 +3090,44 @@
       <c r="AH43" s="17"/>
       <c r="AI43" s="17"/>
       <c r="AJ43" s="17"/>
-      <c r="AK43" s="15"/>
+      <c r="AK43" s="17"/>
       <c r="AL43" s="15"/>
       <c r="AM43" s="15"/>
       <c r="AN43" s="15"/>
       <c r="AO43" s="15"/>
       <c r="AP43" s="15"/>
       <c r="AQ43" s="15"/>
-    </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR43" s="15"/>
+    </row>
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B44" s="19"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
       <c r="F44" s="19"/>
-      <c r="G44" s="17"/>
+      <c r="G44" s="27"/>
       <c r="H44" s="17"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="19"/>
       <c r="K44" s="17"/>
       <c r="L44" s="17"/>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="19"/>
       <c r="Q44" s="17"/>
       <c r="R44" s="17"/>
       <c r="S44" s="17"/>
       <c r="T44" s="17"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="19"/>
       <c r="W44" s="17"/>
       <c r="X44" s="17"/>
       <c r="Y44" s="17"/>
       <c r="Z44" s="17"/>
       <c r="AA44" s="17"/>
-      <c r="AB44" s="19"/>
-      <c r="AC44" s="17"/>
+      <c r="AB44" s="17"/>
+      <c r="AC44" s="19"/>
       <c r="AD44" s="17"/>
       <c r="AE44" s="17"/>
       <c r="AF44" s="17"/>
@@ -3073,43 +3135,44 @@
       <c r="AH44" s="17"/>
       <c r="AI44" s="17"/>
       <c r="AJ44" s="17"/>
-      <c r="AK44" s="15"/>
+      <c r="AK44" s="17"/>
       <c r="AL44" s="15"/>
       <c r="AM44" s="15"/>
       <c r="AN44" s="15"/>
       <c r="AO44" s="15"/>
       <c r="AP44" s="15"/>
       <c r="AQ44" s="15"/>
-    </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR44" s="15"/>
+    </row>
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B45" s="19"/>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
       <c r="F45" s="19"/>
-      <c r="G45" s="17"/>
+      <c r="G45" s="27"/>
       <c r="H45" s="17"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="19"/>
       <c r="K45" s="17"/>
       <c r="L45" s="17"/>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="19"/>
       <c r="Q45" s="17"/>
       <c r="R45" s="17"/>
       <c r="S45" s="17"/>
       <c r="T45" s="17"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="17"/>
+      <c r="U45" s="17"/>
+      <c r="V45" s="19"/>
       <c r="W45" s="17"/>
       <c r="X45" s="17"/>
       <c r="Y45" s="17"/>
       <c r="Z45" s="17"/>
       <c r="AA45" s="17"/>
-      <c r="AB45" s="19"/>
-      <c r="AC45" s="17"/>
+      <c r="AB45" s="17"/>
+      <c r="AC45" s="19"/>
       <c r="AD45" s="17"/>
       <c r="AE45" s="17"/>
       <c r="AF45" s="17"/>
@@ -3117,43 +3180,44 @@
       <c r="AH45" s="17"/>
       <c r="AI45" s="17"/>
       <c r="AJ45" s="17"/>
-      <c r="AK45" s="15"/>
+      <c r="AK45" s="17"/>
       <c r="AL45" s="15"/>
       <c r="AM45" s="15"/>
       <c r="AN45" s="15"/>
       <c r="AO45" s="15"/>
       <c r="AP45" s="15"/>
       <c r="AQ45" s="15"/>
-    </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR45" s="15"/>
+    </row>
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B46" s="19"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
       <c r="F46" s="19"/>
-      <c r="G46" s="17"/>
+      <c r="G46" s="27"/>
       <c r="H46" s="17"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="19"/>
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
-      <c r="O46" s="19"/>
-      <c r="P46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="19"/>
       <c r="Q46" s="17"/>
       <c r="R46" s="17"/>
       <c r="S46" s="17"/>
       <c r="T46" s="17"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="17"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="19"/>
       <c r="W46" s="17"/>
       <c r="X46" s="17"/>
       <c r="Y46" s="17"/>
       <c r="Z46" s="17"/>
       <c r="AA46" s="17"/>
-      <c r="AB46" s="19"/>
-      <c r="AC46" s="17"/>
+      <c r="AB46" s="17"/>
+      <c r="AC46" s="19"/>
       <c r="AD46" s="17"/>
       <c r="AE46" s="17"/>
       <c r="AF46" s="17"/>
@@ -3161,43 +3225,44 @@
       <c r="AH46" s="17"/>
       <c r="AI46" s="17"/>
       <c r="AJ46" s="17"/>
-      <c r="AK46" s="15"/>
+      <c r="AK46" s="17"/>
       <c r="AL46" s="15"/>
       <c r="AM46" s="15"/>
       <c r="AN46" s="15"/>
       <c r="AO46" s="15"/>
       <c r="AP46" s="15"/>
       <c r="AQ46" s="15"/>
-    </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR46" s="15"/>
+    </row>
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B47" s="19"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
       <c r="F47" s="19"/>
-      <c r="G47" s="17"/>
+      <c r="G47" s="27"/>
       <c r="H47" s="17"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="19"/>
       <c r="K47" s="17"/>
       <c r="L47" s="17"/>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
-      <c r="O47" s="19"/>
-      <c r="P47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="19"/>
       <c r="Q47" s="17"/>
       <c r="R47" s="17"/>
       <c r="S47" s="17"/>
       <c r="T47" s="17"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="19"/>
       <c r="W47" s="17"/>
       <c r="X47" s="17"/>
       <c r="Y47" s="17"/>
       <c r="Z47" s="17"/>
       <c r="AA47" s="17"/>
-      <c r="AB47" s="19"/>
-      <c r="AC47" s="17"/>
+      <c r="AB47" s="17"/>
+      <c r="AC47" s="19"/>
       <c r="AD47" s="17"/>
       <c r="AE47" s="17"/>
       <c r="AF47" s="17"/>
@@ -3205,43 +3270,44 @@
       <c r="AH47" s="17"/>
       <c r="AI47" s="17"/>
       <c r="AJ47" s="17"/>
-      <c r="AK47" s="15"/>
+      <c r="AK47" s="17"/>
       <c r="AL47" s="15"/>
       <c r="AM47" s="15"/>
       <c r="AN47" s="15"/>
       <c r="AO47" s="15"/>
       <c r="AP47" s="15"/>
       <c r="AQ47" s="15"/>
-    </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR47" s="15"/>
+    </row>
+    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B48" s="19"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
       <c r="F48" s="19"/>
-      <c r="G48" s="17"/>
+      <c r="G48" s="27"/>
       <c r="H48" s="17"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="19"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
-      <c r="O48" s="19"/>
-      <c r="P48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="19"/>
       <c r="Q48" s="17"/>
       <c r="R48" s="17"/>
       <c r="S48" s="17"/>
       <c r="T48" s="17"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="19"/>
       <c r="W48" s="17"/>
       <c r="X48" s="17"/>
       <c r="Y48" s="17"/>
       <c r="Z48" s="17"/>
       <c r="AA48" s="17"/>
-      <c r="AB48" s="19"/>
-      <c r="AC48" s="17"/>
+      <c r="AB48" s="17"/>
+      <c r="AC48" s="19"/>
       <c r="AD48" s="17"/>
       <c r="AE48" s="17"/>
       <c r="AF48" s="17"/>
@@ -3249,43 +3315,44 @@
       <c r="AH48" s="17"/>
       <c r="AI48" s="17"/>
       <c r="AJ48" s="17"/>
-      <c r="AK48" s="15"/>
+      <c r="AK48" s="17"/>
       <c r="AL48" s="15"/>
       <c r="AM48" s="15"/>
       <c r="AN48" s="15"/>
       <c r="AO48" s="15"/>
       <c r="AP48" s="15"/>
       <c r="AQ48" s="15"/>
-    </row>
-    <row r="49" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR48" s="15"/>
+    </row>
+    <row r="49" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B49" s="19"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
       <c r="E49" s="17"/>
       <c r="F49" s="19"/>
-      <c r="G49" s="17"/>
+      <c r="G49" s="27"/>
       <c r="H49" s="17"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="19"/>
       <c r="K49" s="17"/>
       <c r="L49" s="17"/>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
-      <c r="O49" s="19"/>
-      <c r="P49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="19"/>
       <c r="Q49" s="17"/>
       <c r="R49" s="17"/>
       <c r="S49" s="17"/>
       <c r="T49" s="17"/>
-      <c r="U49" s="19"/>
-      <c r="V49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="19"/>
       <c r="W49" s="17"/>
       <c r="X49" s="17"/>
       <c r="Y49" s="17"/>
       <c r="Z49" s="17"/>
       <c r="AA49" s="17"/>
-      <c r="AB49" s="19"/>
-      <c r="AC49" s="17"/>
+      <c r="AB49" s="17"/>
+      <c r="AC49" s="19"/>
       <c r="AD49" s="17"/>
       <c r="AE49" s="17"/>
       <c r="AF49" s="17"/>
@@ -3293,43 +3360,44 @@
       <c r="AH49" s="17"/>
       <c r="AI49" s="17"/>
       <c r="AJ49" s="17"/>
-      <c r="AK49" s="15"/>
+      <c r="AK49" s="17"/>
       <c r="AL49" s="15"/>
       <c r="AM49" s="15"/>
       <c r="AN49" s="15"/>
       <c r="AO49" s="15"/>
       <c r="AP49" s="15"/>
       <c r="AQ49" s="15"/>
-    </row>
-    <row r="50" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR49" s="15"/>
+    </row>
+    <row r="50" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B50" s="19"/>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
       <c r="F50" s="19"/>
-      <c r="G50" s="17"/>
+      <c r="G50" s="27"/>
       <c r="H50" s="17"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="19"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="19"/>
       <c r="Q50" s="17"/>
       <c r="R50" s="17"/>
       <c r="S50" s="17"/>
       <c r="T50" s="17"/>
-      <c r="U50" s="19"/>
-      <c r="V50" s="17"/>
+      <c r="U50" s="17"/>
+      <c r="V50" s="19"/>
       <c r="W50" s="17"/>
       <c r="X50" s="17"/>
       <c r="Y50" s="17"/>
       <c r="Z50" s="17"/>
       <c r="AA50" s="17"/>
-      <c r="AB50" s="19"/>
-      <c r="AC50" s="17"/>
+      <c r="AB50" s="17"/>
+      <c r="AC50" s="19"/>
       <c r="AD50" s="17"/>
       <c r="AE50" s="17"/>
       <c r="AF50" s="17"/>
@@ -3337,43 +3405,44 @@
       <c r="AH50" s="17"/>
       <c r="AI50" s="17"/>
       <c r="AJ50" s="17"/>
-      <c r="AK50" s="15"/>
+      <c r="AK50" s="17"/>
       <c r="AL50" s="15"/>
       <c r="AM50" s="15"/>
       <c r="AN50" s="15"/>
       <c r="AO50" s="15"/>
       <c r="AP50" s="15"/>
       <c r="AQ50" s="15"/>
-    </row>
-    <row r="51" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR50" s="15"/>
+    </row>
+    <row r="51" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B51" s="19"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
       <c r="F51" s="19"/>
-      <c r="G51" s="17"/>
+      <c r="G51" s="27"/>
       <c r="H51" s="17"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="19"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="19"/>
       <c r="Q51" s="17"/>
       <c r="R51" s="17"/>
       <c r="S51" s="17"/>
       <c r="T51" s="17"/>
-      <c r="U51" s="19"/>
-      <c r="V51" s="17"/>
+      <c r="U51" s="17"/>
+      <c r="V51" s="19"/>
       <c r="W51" s="17"/>
       <c r="X51" s="17"/>
       <c r="Y51" s="17"/>
       <c r="Z51" s="17"/>
       <c r="AA51" s="17"/>
-      <c r="AB51" s="19"/>
-      <c r="AC51" s="17"/>
+      <c r="AB51" s="17"/>
+      <c r="AC51" s="19"/>
       <c r="AD51" s="17"/>
       <c r="AE51" s="17"/>
       <c r="AF51" s="17"/>
@@ -3381,43 +3450,44 @@
       <c r="AH51" s="17"/>
       <c r="AI51" s="17"/>
       <c r="AJ51" s="17"/>
-      <c r="AK51" s="15"/>
+      <c r="AK51" s="17"/>
       <c r="AL51" s="15"/>
       <c r="AM51" s="15"/>
       <c r="AN51" s="15"/>
       <c r="AO51" s="15"/>
       <c r="AP51" s="15"/>
       <c r="AQ51" s="15"/>
-    </row>
-    <row r="52" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR51" s="15"/>
+    </row>
+    <row r="52" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B52" s="19"/>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
       <c r="E52" s="17"/>
       <c r="F52" s="19"/>
-      <c r="G52" s="17"/>
+      <c r="G52" s="27"/>
       <c r="H52" s="17"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="19"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
-      <c r="O52" s="19"/>
-      <c r="P52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="19"/>
       <c r="Q52" s="17"/>
       <c r="R52" s="17"/>
       <c r="S52" s="17"/>
       <c r="T52" s="17"/>
-      <c r="U52" s="19"/>
-      <c r="V52" s="17"/>
+      <c r="U52" s="17"/>
+      <c r="V52" s="19"/>
       <c r="W52" s="17"/>
       <c r="X52" s="17"/>
       <c r="Y52" s="17"/>
       <c r="Z52" s="17"/>
       <c r="AA52" s="17"/>
-      <c r="AB52" s="19"/>
-      <c r="AC52" s="17"/>
+      <c r="AB52" s="17"/>
+      <c r="AC52" s="19"/>
       <c r="AD52" s="17"/>
       <c r="AE52" s="17"/>
       <c r="AF52" s="17"/>
@@ -3425,43 +3495,44 @@
       <c r="AH52" s="17"/>
       <c r="AI52" s="17"/>
       <c r="AJ52" s="17"/>
-      <c r="AK52" s="15"/>
+      <c r="AK52" s="17"/>
       <c r="AL52" s="15"/>
       <c r="AM52" s="15"/>
       <c r="AN52" s="15"/>
       <c r="AO52" s="15"/>
       <c r="AP52" s="15"/>
       <c r="AQ52" s="15"/>
-    </row>
-    <row r="53" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR52" s="15"/>
+    </row>
+    <row r="53" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B53" s="19"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
       <c r="F53" s="19"/>
-      <c r="G53" s="17"/>
+      <c r="G53" s="27"/>
       <c r="H53" s="17"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="19"/>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
-      <c r="O53" s="19"/>
-      <c r="P53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="19"/>
       <c r="Q53" s="17"/>
       <c r="R53" s="17"/>
       <c r="S53" s="17"/>
       <c r="T53" s="17"/>
-      <c r="U53" s="19"/>
-      <c r="V53" s="17"/>
+      <c r="U53" s="17"/>
+      <c r="V53" s="19"/>
       <c r="W53" s="17"/>
       <c r="X53" s="17"/>
       <c r="Y53" s="17"/>
       <c r="Z53" s="17"/>
       <c r="AA53" s="17"/>
-      <c r="AB53" s="19"/>
-      <c r="AC53" s="17"/>
+      <c r="AB53" s="17"/>
+      <c r="AC53" s="19"/>
       <c r="AD53" s="17"/>
       <c r="AE53" s="17"/>
       <c r="AF53" s="17"/>
@@ -3469,43 +3540,44 @@
       <c r="AH53" s="17"/>
       <c r="AI53" s="17"/>
       <c r="AJ53" s="17"/>
-      <c r="AK53" s="15"/>
+      <c r="AK53" s="17"/>
       <c r="AL53" s="15"/>
       <c r="AM53" s="15"/>
       <c r="AN53" s="15"/>
       <c r="AO53" s="15"/>
       <c r="AP53" s="15"/>
       <c r="AQ53" s="15"/>
-    </row>
-    <row r="54" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR53" s="15"/>
+    </row>
+    <row r="54" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B54" s="19"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
       <c r="F54" s="19"/>
-      <c r="G54" s="17"/>
+      <c r="G54" s="27"/>
       <c r="H54" s="17"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="19"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
       <c r="M54" s="17"/>
       <c r="N54" s="17"/>
-      <c r="O54" s="19"/>
-      <c r="P54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="19"/>
       <c r="Q54" s="17"/>
       <c r="R54" s="17"/>
       <c r="S54" s="17"/>
       <c r="T54" s="17"/>
-      <c r="U54" s="19"/>
-      <c r="V54" s="17"/>
+      <c r="U54" s="17"/>
+      <c r="V54" s="19"/>
       <c r="W54" s="17"/>
       <c r="X54" s="17"/>
       <c r="Y54" s="17"/>
       <c r="Z54" s="17"/>
       <c r="AA54" s="17"/>
-      <c r="AB54" s="19"/>
-      <c r="AC54" s="17"/>
+      <c r="AB54" s="17"/>
+      <c r="AC54" s="19"/>
       <c r="AD54" s="17"/>
       <c r="AE54" s="17"/>
       <c r="AF54" s="17"/>
@@ -3513,43 +3585,44 @@
       <c r="AH54" s="17"/>
       <c r="AI54" s="17"/>
       <c r="AJ54" s="17"/>
-      <c r="AK54" s="15"/>
+      <c r="AK54" s="17"/>
       <c r="AL54" s="15"/>
       <c r="AM54" s="15"/>
       <c r="AN54" s="15"/>
       <c r="AO54" s="15"/>
       <c r="AP54" s="15"/>
       <c r="AQ54" s="15"/>
-    </row>
-    <row r="55" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR54" s="15"/>
+    </row>
+    <row r="55" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B55" s="19"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
       <c r="F55" s="19"/>
-      <c r="G55" s="17"/>
+      <c r="G55" s="27"/>
       <c r="H55" s="17"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="19"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
-      <c r="O55" s="19"/>
-      <c r="P55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="19"/>
       <c r="Q55" s="17"/>
       <c r="R55" s="17"/>
       <c r="S55" s="17"/>
       <c r="T55" s="17"/>
-      <c r="U55" s="19"/>
-      <c r="V55" s="17"/>
+      <c r="U55" s="17"/>
+      <c r="V55" s="19"/>
       <c r="W55" s="17"/>
       <c r="X55" s="17"/>
       <c r="Y55" s="17"/>
       <c r="Z55" s="17"/>
       <c r="AA55" s="17"/>
-      <c r="AB55" s="19"/>
-      <c r="AC55" s="17"/>
+      <c r="AB55" s="17"/>
+      <c r="AC55" s="19"/>
       <c r="AD55" s="17"/>
       <c r="AE55" s="17"/>
       <c r="AF55" s="17"/>
@@ -3557,43 +3630,44 @@
       <c r="AH55" s="17"/>
       <c r="AI55" s="17"/>
       <c r="AJ55" s="17"/>
-      <c r="AK55" s="15"/>
+      <c r="AK55" s="17"/>
       <c r="AL55" s="15"/>
       <c r="AM55" s="15"/>
       <c r="AN55" s="15"/>
       <c r="AO55" s="15"/>
       <c r="AP55" s="15"/>
       <c r="AQ55" s="15"/>
-    </row>
-    <row r="56" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR55" s="15"/>
+    </row>
+    <row r="56" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B56" s="19"/>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
       <c r="F56" s="19"/>
-      <c r="G56" s="17"/>
+      <c r="G56" s="27"/>
       <c r="H56" s="17"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="19"/>
       <c r="K56" s="17"/>
       <c r="L56" s="17"/>
       <c r="M56" s="17"/>
       <c r="N56" s="17"/>
-      <c r="O56" s="19"/>
-      <c r="P56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="19"/>
       <c r="Q56" s="17"/>
       <c r="R56" s="17"/>
       <c r="S56" s="17"/>
       <c r="T56" s="17"/>
-      <c r="U56" s="19"/>
-      <c r="V56" s="17"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="19"/>
       <c r="W56" s="17"/>
       <c r="X56" s="17"/>
       <c r="Y56" s="17"/>
       <c r="Z56" s="17"/>
       <c r="AA56" s="17"/>
-      <c r="AB56" s="19"/>
-      <c r="AC56" s="17"/>
+      <c r="AB56" s="17"/>
+      <c r="AC56" s="19"/>
       <c r="AD56" s="17"/>
       <c r="AE56" s="17"/>
       <c r="AF56" s="17"/>
@@ -3601,43 +3675,44 @@
       <c r="AH56" s="17"/>
       <c r="AI56" s="17"/>
       <c r="AJ56" s="17"/>
-      <c r="AK56" s="15"/>
+      <c r="AK56" s="17"/>
       <c r="AL56" s="15"/>
       <c r="AM56" s="15"/>
       <c r="AN56" s="15"/>
       <c r="AO56" s="15"/>
       <c r="AP56" s="15"/>
       <c r="AQ56" s="15"/>
-    </row>
-    <row r="57" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR56" s="15"/>
+    </row>
+    <row r="57" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B57" s="19"/>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
       <c r="F57" s="19"/>
-      <c r="G57" s="17"/>
+      <c r="G57" s="27"/>
       <c r="H57" s="17"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="19"/>
       <c r="K57" s="17"/>
       <c r="L57" s="17"/>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
-      <c r="O57" s="19"/>
-      <c r="P57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="19"/>
       <c r="Q57" s="17"/>
       <c r="R57" s="17"/>
       <c r="S57" s="17"/>
       <c r="T57" s="17"/>
-      <c r="U57" s="19"/>
-      <c r="V57" s="17"/>
+      <c r="U57" s="17"/>
+      <c r="V57" s="19"/>
       <c r="W57" s="17"/>
       <c r="X57" s="17"/>
       <c r="Y57" s="17"/>
       <c r="Z57" s="17"/>
       <c r="AA57" s="17"/>
-      <c r="AB57" s="19"/>
-      <c r="AC57" s="17"/>
+      <c r="AB57" s="17"/>
+      <c r="AC57" s="19"/>
       <c r="AD57" s="17"/>
       <c r="AE57" s="17"/>
       <c r="AF57" s="17"/>
@@ -3645,43 +3720,44 @@
       <c r="AH57" s="17"/>
       <c r="AI57" s="17"/>
       <c r="AJ57" s="17"/>
-      <c r="AK57" s="15"/>
+      <c r="AK57" s="17"/>
       <c r="AL57" s="15"/>
       <c r="AM57" s="15"/>
       <c r="AN57" s="15"/>
       <c r="AO57" s="15"/>
       <c r="AP57" s="15"/>
       <c r="AQ57" s="15"/>
-    </row>
-    <row r="58" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR57" s="15"/>
+    </row>
+    <row r="58" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B58" s="19"/>
       <c r="C58" s="17"/>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
       <c r="F58" s="19"/>
-      <c r="G58" s="17"/>
+      <c r="G58" s="27"/>
       <c r="H58" s="17"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="19"/>
       <c r="K58" s="17"/>
       <c r="L58" s="17"/>
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
-      <c r="O58" s="19"/>
-      <c r="P58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="19"/>
       <c r="Q58" s="17"/>
       <c r="R58" s="17"/>
       <c r="S58" s="17"/>
       <c r="T58" s="17"/>
-      <c r="U58" s="19"/>
-      <c r="V58" s="17"/>
+      <c r="U58" s="17"/>
+      <c r="V58" s="19"/>
       <c r="W58" s="17"/>
       <c r="X58" s="17"/>
       <c r="Y58" s="17"/>
       <c r="Z58" s="17"/>
       <c r="AA58" s="17"/>
-      <c r="AB58" s="19"/>
-      <c r="AC58" s="17"/>
+      <c r="AB58" s="17"/>
+      <c r="AC58" s="19"/>
       <c r="AD58" s="17"/>
       <c r="AE58" s="17"/>
       <c r="AF58" s="17"/>
@@ -3689,43 +3765,44 @@
       <c r="AH58" s="17"/>
       <c r="AI58" s="17"/>
       <c r="AJ58" s="17"/>
-      <c r="AK58" s="15"/>
+      <c r="AK58" s="17"/>
       <c r="AL58" s="15"/>
       <c r="AM58" s="15"/>
       <c r="AN58" s="15"/>
       <c r="AO58" s="15"/>
       <c r="AP58" s="15"/>
       <c r="AQ58" s="15"/>
-    </row>
-    <row r="59" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AR58" s="15"/>
+    </row>
+    <row r="59" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B59" s="20"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="20"/>
-      <c r="G59" s="2"/>
+      <c r="G59" s="28"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="20"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
-      <c r="O59" s="20"/>
-      <c r="P59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="20"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
-      <c r="U59" s="20"/>
-      <c r="V59" s="2"/>
+      <c r="U59" s="2"/>
+      <c r="V59" s="20"/>
       <c r="W59" s="2"/>
       <c r="X59" s="2"/>
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
       <c r="AA59" s="2"/>
-      <c r="AB59" s="20"/>
-      <c r="AC59" s="2"/>
+      <c r="AB59" s="2"/>
+      <c r="AC59" s="20"/>
       <c r="AD59" s="2"/>
       <c r="AE59" s="2"/>
       <c r="AF59" s="2"/>
@@ -3733,36 +3810,37 @@
       <c r="AH59" s="2"/>
       <c r="AI59" s="2"/>
       <c r="AJ59" s="2"/>
-    </row>
-    <row r="60" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AK59" s="2"/>
+    </row>
+    <row r="60" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B60" s="20"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="20"/>
-      <c r="G60" s="2"/>
+      <c r="G60" s="28"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="20"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
-      <c r="O60" s="20"/>
-      <c r="P60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="20"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
-      <c r="U60" s="20"/>
-      <c r="V60" s="2"/>
+      <c r="U60" s="2"/>
+      <c r="V60" s="20"/>
       <c r="W60" s="2"/>
       <c r="X60" s="2"/>
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
       <c r="AA60" s="2"/>
-      <c r="AB60" s="20"/>
-      <c r="AC60" s="2"/>
+      <c r="AB60" s="2"/>
+      <c r="AC60" s="20"/>
       <c r="AD60" s="2"/>
       <c r="AE60" s="2"/>
       <c r="AF60" s="2"/>
@@ -3770,36 +3848,37 @@
       <c r="AH60" s="2"/>
       <c r="AI60" s="2"/>
       <c r="AJ60" s="2"/>
-    </row>
-    <row r="61" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AK60" s="2"/>
+    </row>
+    <row r="61" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B61" s="20"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="20"/>
-      <c r="G61" s="2"/>
+      <c r="G61" s="28"/>
       <c r="H61" s="2"/>
-      <c r="I61" s="20"/>
-      <c r="J61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="20"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
-      <c r="O61" s="20"/>
-      <c r="P61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="20"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
-      <c r="U61" s="20"/>
-      <c r="V61" s="2"/>
+      <c r="U61" s="2"/>
+      <c r="V61" s="20"/>
       <c r="W61" s="2"/>
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
       <c r="AA61" s="2"/>
-      <c r="AB61" s="20"/>
-      <c r="AC61" s="2"/>
+      <c r="AB61" s="2"/>
+      <c r="AC61" s="20"/>
       <c r="AD61" s="2"/>
       <c r="AE61" s="2"/>
       <c r="AF61" s="2"/>
@@ -3807,36 +3886,37 @@
       <c r="AH61" s="2"/>
       <c r="AI61" s="2"/>
       <c r="AJ61" s="2"/>
-    </row>
-    <row r="62" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AK61" s="2"/>
+    </row>
+    <row r="62" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B62" s="20"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="20"/>
-      <c r="G62" s="2"/>
+      <c r="G62" s="28"/>
       <c r="H62" s="2"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="20"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
-      <c r="O62" s="20"/>
-      <c r="P62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="20"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
-      <c r="U62" s="20"/>
-      <c r="V62" s="2"/>
+      <c r="U62" s="2"/>
+      <c r="V62" s="20"/>
       <c r="W62" s="2"/>
       <c r="X62" s="2"/>
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
       <c r="AA62" s="2"/>
-      <c r="AB62" s="20"/>
-      <c r="AC62" s="2"/>
+      <c r="AB62" s="2"/>
+      <c r="AC62" s="20"/>
       <c r="AD62" s="2"/>
       <c r="AE62" s="2"/>
       <c r="AF62" s="2"/>
@@ -3844,36 +3924,37 @@
       <c r="AH62" s="2"/>
       <c r="AI62" s="2"/>
       <c r="AJ62" s="2"/>
-    </row>
-    <row r="63" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AK62" s="2"/>
+    </row>
+    <row r="63" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B63" s="20"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="20"/>
-      <c r="G63" s="2"/>
+      <c r="G63" s="28"/>
       <c r="H63" s="2"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="20"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
-      <c r="O63" s="20"/>
-      <c r="P63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="20"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
-      <c r="U63" s="20"/>
-      <c r="V63" s="2"/>
+      <c r="U63" s="2"/>
+      <c r="V63" s="20"/>
       <c r="W63" s="2"/>
       <c r="X63" s="2"/>
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
       <c r="AA63" s="2"/>
-      <c r="AB63" s="20"/>
-      <c r="AC63" s="2"/>
+      <c r="AB63" s="2"/>
+      <c r="AC63" s="20"/>
       <c r="AD63" s="2"/>
       <c r="AE63" s="2"/>
       <c r="AF63" s="2"/>
@@ -3881,36 +3962,37 @@
       <c r="AH63" s="2"/>
       <c r="AI63" s="2"/>
       <c r="AJ63" s="2"/>
-    </row>
-    <row r="64" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="AK63" s="2"/>
+    </row>
+    <row r="64" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B64" s="20"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="20"/>
-      <c r="G64" s="2"/>
+      <c r="G64" s="28"/>
       <c r="H64" s="2"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="20"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
-      <c r="O64" s="20"/>
-      <c r="P64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="20"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
-      <c r="U64" s="20"/>
-      <c r="V64" s="2"/>
+      <c r="U64" s="2"/>
+      <c r="V64" s="20"/>
       <c r="W64" s="2"/>
       <c r="X64" s="2"/>
       <c r="Y64" s="2"/>
       <c r="Z64" s="2"/>
       <c r="AA64" s="2"/>
-      <c r="AB64" s="20"/>
-      <c r="AC64" s="2"/>
+      <c r="AB64" s="2"/>
+      <c r="AC64" s="20"/>
       <c r="AD64" s="2"/>
       <c r="AE64" s="2"/>
       <c r="AF64" s="2"/>
@@ -3918,36 +4000,37 @@
       <c r="AH64" s="2"/>
       <c r="AI64" s="2"/>
       <c r="AJ64" s="2"/>
-    </row>
-    <row r="65" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK64" s="2"/>
+    </row>
+    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B65" s="20"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="20"/>
-      <c r="G65" s="2"/>
+      <c r="G65" s="28"/>
       <c r="H65" s="2"/>
-      <c r="I65" s="20"/>
-      <c r="J65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="20"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
-      <c r="O65" s="20"/>
-      <c r="P65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="20"/>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
-      <c r="U65" s="20"/>
-      <c r="V65" s="2"/>
+      <c r="U65" s="2"/>
+      <c r="V65" s="20"/>
       <c r="W65" s="2"/>
       <c r="X65" s="2"/>
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
       <c r="AA65" s="2"/>
-      <c r="AB65" s="20"/>
-      <c r="AC65" s="2"/>
+      <c r="AB65" s="2"/>
+      <c r="AC65" s="20"/>
       <c r="AD65" s="2"/>
       <c r="AE65" s="2"/>
       <c r="AF65" s="2"/>
@@ -3955,36 +4038,37 @@
       <c r="AH65" s="2"/>
       <c r="AI65" s="2"/>
       <c r="AJ65" s="2"/>
-    </row>
-    <row r="66" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK65" s="2"/>
+    </row>
+    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B66" s="20"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="20"/>
-      <c r="G66" s="2"/>
+      <c r="G66" s="28"/>
       <c r="H66" s="2"/>
-      <c r="I66" s="20"/>
-      <c r="J66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="20"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
-      <c r="O66" s="20"/>
-      <c r="P66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="20"/>
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
-      <c r="U66" s="20"/>
-      <c r="V66" s="2"/>
+      <c r="U66" s="2"/>
+      <c r="V66" s="20"/>
       <c r="W66" s="2"/>
       <c r="X66" s="2"/>
       <c r="Y66" s="2"/>
       <c r="Z66" s="2"/>
       <c r="AA66" s="2"/>
-      <c r="AB66" s="20"/>
-      <c r="AC66" s="2"/>
+      <c r="AB66" s="2"/>
+      <c r="AC66" s="20"/>
       <c r="AD66" s="2"/>
       <c r="AE66" s="2"/>
       <c r="AF66" s="2"/>
@@ -3992,36 +4076,37 @@
       <c r="AH66" s="2"/>
       <c r="AI66" s="2"/>
       <c r="AJ66" s="2"/>
-    </row>
-    <row r="67" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK66" s="2"/>
+    </row>
+    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B67" s="20"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="20"/>
-      <c r="G67" s="2"/>
+      <c r="G67" s="28"/>
       <c r="H67" s="2"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="20"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
-      <c r="O67" s="20"/>
-      <c r="P67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="20"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
-      <c r="U67" s="20"/>
-      <c r="V67" s="2"/>
+      <c r="U67" s="2"/>
+      <c r="V67" s="20"/>
       <c r="W67" s="2"/>
       <c r="X67" s="2"/>
       <c r="Y67" s="2"/>
       <c r="Z67" s="2"/>
       <c r="AA67" s="2"/>
-      <c r="AB67" s="20"/>
-      <c r="AC67" s="2"/>
+      <c r="AB67" s="2"/>
+      <c r="AC67" s="20"/>
       <c r="AD67" s="2"/>
       <c r="AE67" s="2"/>
       <c r="AF67" s="2"/>
@@ -4029,36 +4114,37 @@
       <c r="AH67" s="2"/>
       <c r="AI67" s="2"/>
       <c r="AJ67" s="2"/>
-    </row>
-    <row r="68" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK67" s="2"/>
+    </row>
+    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B68" s="20"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="20"/>
-      <c r="G68" s="2"/>
+      <c r="G68" s="28"/>
       <c r="H68" s="2"/>
-      <c r="I68" s="20"/>
-      <c r="J68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="20"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
-      <c r="O68" s="20"/>
-      <c r="P68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="20"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
-      <c r="U68" s="20"/>
-      <c r="V68" s="2"/>
+      <c r="U68" s="2"/>
+      <c r="V68" s="20"/>
       <c r="W68" s="2"/>
       <c r="X68" s="2"/>
       <c r="Y68" s="2"/>
       <c r="Z68" s="2"/>
       <c r="AA68" s="2"/>
-      <c r="AB68" s="20"/>
-      <c r="AC68" s="2"/>
+      <c r="AB68" s="2"/>
+      <c r="AC68" s="20"/>
       <c r="AD68" s="2"/>
       <c r="AE68" s="2"/>
       <c r="AF68" s="2"/>
@@ -4066,49 +4152,50 @@
       <c r="AH68" s="2"/>
       <c r="AI68" s="2"/>
       <c r="AJ68" s="2"/>
+      <c r="AK68" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:AJ22 B24:AJ68">
+  <conditionalFormatting sqref="B2:AK22 B24:AK68">
     <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P10:R13 P16:R22 X16:X22 X24:X36 P24:R36">
+  <conditionalFormatting sqref="Q10:S13 Q16:S22 Y16:Y22 Y24:Y36 Q24:S36">
     <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P7:R8">
+  <conditionalFormatting sqref="Q7:S8">
     <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P9:R9">
+  <conditionalFormatting sqref="Q9:S9">
     <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X7:X8">
+  <conditionalFormatting sqref="Y7:Y8">
     <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X9">
+  <conditionalFormatting sqref="Y9">
     <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X10:X13">
+  <conditionalFormatting sqref="Y10:Y13">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:AJ23">
+  <conditionalFormatting sqref="B23:AK23">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X23 P23:R23">
+  <conditionalFormatting sqref="Y23 Q23:S23">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>

</xml_diff>